<commit_message>
Commit Decide MLR and RNN
</commit_message>
<xml_diff>
--- a/MergedFile.xlsx
+++ b/MergedFile.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\CiliLado\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F771228-D237-4F61-A15B-0C0DC516A7A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1BB9BA2-87B3-4907-941C-11774742FDC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -175,7 +175,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -185,7 +185,11 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,14 +531,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Y185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E149" sqref="E149"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12" style="2" customWidth="1"/>
-    <col min="2" max="23" width="12" customWidth="1"/>
+    <col min="2" max="19" width="12" customWidth="1"/>
+    <col min="20" max="20" width="12" style="9" customWidth="1"/>
+    <col min="21" max="23" width="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
@@ -595,7 +601,7 @@
       <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
       <c r="U1" s="1" t="s">
@@ -672,7 +678,7 @@
       <c r="S2" s="3">
         <v>0</v>
       </c>
-      <c r="T2" s="3">
+      <c r="T2" s="8">
         <v>0</v>
       </c>
       <c r="U2" s="5">
@@ -749,7 +755,7 @@
       <c r="S3" s="3">
         <v>1</v>
       </c>
-      <c r="T3" s="3">
+      <c r="T3" s="8">
         <v>58.9</v>
       </c>
       <c r="U3" s="5">
@@ -826,7 +832,7 @@
       <c r="S4" s="3">
         <v>0</v>
       </c>
-      <c r="T4" s="3">
+      <c r="T4" s="8">
         <v>0</v>
       </c>
       <c r="U4" s="5">
@@ -903,7 +909,7 @@
       <c r="S5" s="3">
         <v>0</v>
       </c>
-      <c r="T5" s="3">
+      <c r="T5" s="8">
         <v>0</v>
       </c>
       <c r="U5" s="5">
@@ -980,7 +986,7 @@
       <c r="S6" s="3">
         <v>0</v>
       </c>
-      <c r="T6" s="3">
+      <c r="T6" s="8">
         <v>0</v>
       </c>
       <c r="U6" s="5">
@@ -1057,7 +1063,7 @@
       <c r="S7" s="3">
         <v>0</v>
       </c>
-      <c r="T7" s="3">
+      <c r="T7" s="8">
         <v>0</v>
       </c>
       <c r="U7" s="5">
@@ -1134,7 +1140,7 @@
       <c r="S8" s="3">
         <v>0</v>
       </c>
-      <c r="T8" s="3">
+      <c r="T8" s="8">
         <v>0</v>
       </c>
       <c r="U8" s="5">
@@ -1211,7 +1217,7 @@
       <c r="S9" s="3">
         <v>0</v>
       </c>
-      <c r="T9" s="3">
+      <c r="T9" s="8">
         <v>0</v>
       </c>
       <c r="U9" s="5">
@@ -1288,7 +1294,7 @@
       <c r="S10" s="3">
         <v>0</v>
       </c>
-      <c r="T10" s="3">
+      <c r="T10" s="8">
         <v>0</v>
       </c>
       <c r="U10" s="5">
@@ -1365,7 +1371,7 @@
       <c r="S11" s="3">
         <v>0</v>
       </c>
-      <c r="T11" s="3">
+      <c r="T11" s="8">
         <v>0</v>
       </c>
       <c r="U11" s="5">
@@ -1442,7 +1448,7 @@
       <c r="S12" s="3">
         <v>1</v>
       </c>
-      <c r="T12" s="3">
+      <c r="T12" s="8">
         <v>51.9</v>
       </c>
       <c r="U12" s="5">
@@ -1519,7 +1525,7 @@
       <c r="S13" s="3">
         <v>0</v>
       </c>
-      <c r="T13" s="3">
+      <c r="T13" s="8">
         <v>0</v>
       </c>
       <c r="U13" s="5">
@@ -1596,7 +1602,7 @@
       <c r="S14" s="3">
         <v>0</v>
       </c>
-      <c r="T14" s="3">
+      <c r="T14" s="8">
         <v>0</v>
       </c>
       <c r="U14" s="5">
@@ -1673,7 +1679,7 @@
       <c r="S15" s="3">
         <v>1</v>
       </c>
-      <c r="T15" s="3">
+      <c r="T15" s="8">
         <v>113.4</v>
       </c>
       <c r="U15" s="5">
@@ -1750,7 +1756,7 @@
       <c r="S16" s="3">
         <v>1</v>
       </c>
-      <c r="T16" s="3">
+      <c r="T16" s="8">
         <v>17.899999999999999</v>
       </c>
       <c r="U16" s="5">
@@ -1827,7 +1833,7 @@
       <c r="S17" s="3">
         <v>0</v>
       </c>
-      <c r="T17" s="3">
+      <c r="T17" s="8">
         <v>0</v>
       </c>
       <c r="U17" s="5">
@@ -1904,7 +1910,7 @@
       <c r="S18" s="3">
         <v>1</v>
       </c>
-      <c r="T18" s="3">
+      <c r="T18" s="8">
         <v>17.899999999999999</v>
       </c>
       <c r="U18" s="5">
@@ -1981,7 +1987,7 @@
       <c r="S19" s="3">
         <v>0</v>
       </c>
-      <c r="T19" s="3">
+      <c r="T19" s="8">
         <v>0</v>
       </c>
       <c r="U19" s="5">
@@ -2058,7 +2064,7 @@
       <c r="S20" s="3">
         <v>0</v>
       </c>
-      <c r="T20" s="3">
+      <c r="T20" s="8">
         <v>0</v>
       </c>
       <c r="U20" s="5">
@@ -2135,7 +2141,7 @@
       <c r="S21" s="3">
         <v>0</v>
       </c>
-      <c r="T21" s="3">
+      <c r="T21" s="8">
         <v>0</v>
       </c>
       <c r="U21" s="5">
@@ -2212,7 +2218,7 @@
       <c r="S22" s="3">
         <v>0</v>
       </c>
-      <c r="T22" s="3">
+      <c r="T22" s="8">
         <v>0</v>
       </c>
       <c r="U22" s="5">
@@ -2289,7 +2295,7 @@
       <c r="S23" s="3">
         <v>0</v>
       </c>
-      <c r="T23" s="3">
+      <c r="T23" s="8">
         <v>0</v>
       </c>
       <c r="U23" s="5">
@@ -2366,7 +2372,7 @@
       <c r="S24" s="3">
         <v>0</v>
       </c>
-      <c r="T24" s="3">
+      <c r="T24" s="8">
         <v>0</v>
       </c>
       <c r="U24" s="5">
@@ -2443,7 +2449,7 @@
       <c r="S25" s="3">
         <v>0</v>
       </c>
-      <c r="T25" s="3">
+      <c r="T25" s="8">
         <v>0</v>
       </c>
       <c r="U25" s="5">
@@ -2520,7 +2526,7 @@
       <c r="S26" s="3">
         <v>0</v>
       </c>
-      <c r="T26" s="3">
+      <c r="T26" s="8">
         <v>0</v>
       </c>
       <c r="U26" s="5">
@@ -2597,7 +2603,7 @@
       <c r="S27" s="3">
         <v>0</v>
       </c>
-      <c r="T27" s="3">
+      <c r="T27" s="8">
         <v>0</v>
       </c>
       <c r="U27" s="5">
@@ -2674,7 +2680,7 @@
       <c r="S28" s="3">
         <v>0</v>
       </c>
-      <c r="T28" s="3">
+      <c r="T28" s="8">
         <v>0</v>
       </c>
       <c r="U28" s="5">
@@ -2751,7 +2757,7 @@
       <c r="S29" s="3">
         <v>1</v>
       </c>
-      <c r="T29" s="3">
+      <c r="T29" s="8">
         <v>22.9</v>
       </c>
       <c r="U29" s="5">
@@ -2828,7 +2834,7 @@
       <c r="S30" s="3">
         <v>0</v>
       </c>
-      <c r="T30" s="3">
+      <c r="T30" s="8">
         <v>0</v>
       </c>
       <c r="U30" s="5">
@@ -2905,7 +2911,7 @@
       <c r="S31" s="3">
         <v>0</v>
       </c>
-      <c r="T31" s="3">
+      <c r="T31" s="8">
         <v>0</v>
       </c>
       <c r="U31" s="5">
@@ -2982,7 +2988,7 @@
       <c r="S32" s="3">
         <v>0</v>
       </c>
-      <c r="T32" s="3">
+      <c r="T32" s="8">
         <v>0</v>
       </c>
       <c r="U32" s="5">
@@ -3059,7 +3065,7 @@
       <c r="S33" s="3">
         <v>0</v>
       </c>
-      <c r="T33" s="3">
+      <c r="T33" s="8">
         <v>0</v>
       </c>
       <c r="U33" s="5">
@@ -3136,7 +3142,7 @@
       <c r="S34" s="3">
         <v>0</v>
       </c>
-      <c r="T34" s="3">
+      <c r="T34" s="8">
         <v>0</v>
       </c>
       <c r="U34" s="5">
@@ -3213,7 +3219,7 @@
       <c r="S35" s="3">
         <v>0</v>
       </c>
-      <c r="T35" s="3">
+      <c r="T35" s="8">
         <v>0</v>
       </c>
       <c r="U35" s="5">
@@ -3290,7 +3296,7 @@
       <c r="S36" s="3">
         <v>0</v>
       </c>
-      <c r="T36" s="3">
+      <c r="T36" s="8">
         <v>0</v>
       </c>
       <c r="U36" s="5">
@@ -3367,7 +3373,7 @@
       <c r="S37" s="3">
         <v>1</v>
       </c>
-      <c r="T37" s="3">
+      <c r="T37" s="8">
         <v>22.9</v>
       </c>
       <c r="U37" s="5">
@@ -3444,7 +3450,7 @@
       <c r="S38" s="3">
         <v>0</v>
       </c>
-      <c r="T38" s="3">
+      <c r="T38" s="8">
         <v>0</v>
       </c>
       <c r="U38" s="5">
@@ -3521,7 +3527,7 @@
       <c r="S39" s="3">
         <v>0</v>
       </c>
-      <c r="T39" s="3">
+      <c r="T39" s="8">
         <v>0</v>
       </c>
       <c r="U39" s="5">
@@ -3598,7 +3604,7 @@
       <c r="S40" s="3">
         <v>0</v>
       </c>
-      <c r="T40" s="3">
+      <c r="T40" s="8">
         <v>0</v>
       </c>
       <c r="U40" s="5">
@@ -3675,7 +3681,7 @@
       <c r="S41" s="3">
         <v>0</v>
       </c>
-      <c r="T41" s="3">
+      <c r="T41" s="8">
         <v>0</v>
       </c>
       <c r="U41" s="5">
@@ -3752,7 +3758,7 @@
       <c r="S42" s="3">
         <v>0</v>
       </c>
-      <c r="T42" s="3">
+      <c r="T42" s="8">
         <v>0</v>
       </c>
       <c r="U42" s="5">
@@ -3829,7 +3835,7 @@
       <c r="S43" s="3">
         <v>0</v>
       </c>
-      <c r="T43" s="3">
+      <c r="T43" s="8">
         <v>0</v>
       </c>
       <c r="U43" s="5">
@@ -3906,7 +3912,7 @@
       <c r="S44" s="3">
         <v>0</v>
       </c>
-      <c r="T44" s="3">
+      <c r="T44" s="8">
         <v>0</v>
       </c>
       <c r="U44" s="5">
@@ -3983,7 +3989,7 @@
       <c r="S45" s="3">
         <v>0</v>
       </c>
-      <c r="T45" s="3">
+      <c r="T45" s="8">
         <v>0</v>
       </c>
       <c r="U45" s="5">
@@ -4060,7 +4066,7 @@
       <c r="S46" s="3">
         <v>0</v>
       </c>
-      <c r="T46" s="3">
+      <c r="T46" s="8">
         <v>0</v>
       </c>
       <c r="U46" s="5">
@@ -4137,7 +4143,7 @@
       <c r="S47" s="3">
         <v>0</v>
       </c>
-      <c r="T47" s="3">
+      <c r="T47" s="8">
         <v>0</v>
       </c>
       <c r="U47" s="5">
@@ -4214,7 +4220,7 @@
       <c r="S48" s="3">
         <v>0</v>
       </c>
-      <c r="T48" s="3">
+      <c r="T48" s="8">
         <v>0</v>
       </c>
       <c r="U48" s="5">
@@ -4291,7 +4297,7 @@
       <c r="S49" s="3">
         <v>1</v>
       </c>
-      <c r="T49" s="3">
+      <c r="T49" s="8">
         <v>81.8</v>
       </c>
       <c r="U49" s="5">
@@ -4368,7 +4374,7 @@
       <c r="S50" s="3">
         <v>1</v>
       </c>
-      <c r="T50" s="3">
+      <c r="T50" s="8">
         <v>40.9</v>
       </c>
       <c r="U50" s="5">
@@ -4445,7 +4451,7 @@
       <c r="S51" s="3">
         <v>2</v>
       </c>
-      <c r="T51" s="3">
+      <c r="T51" s="8">
         <v>823.2</v>
       </c>
       <c r="U51" s="5">
@@ -4522,7 +4528,7 @@
       <c r="S52" s="3">
         <v>1</v>
       </c>
-      <c r="T52" s="3">
+      <c r="T52" s="8">
         <v>456.85</v>
       </c>
       <c r="U52" s="5">
@@ -4599,7 +4605,7 @@
       <c r="S53" s="3">
         <v>2</v>
       </c>
-      <c r="T53" s="3">
+      <c r="T53" s="8">
         <v>921.97</v>
       </c>
       <c r="U53" s="5">
@@ -4676,7 +4682,7 @@
       <c r="S54" s="3">
         <v>2</v>
       </c>
-      <c r="T54" s="6">
+      <c r="T54" s="8">
         <v>1491.01</v>
       </c>
       <c r="U54" s="5">
@@ -4753,7 +4759,7 @@
       <c r="S55" s="3">
         <v>2</v>
       </c>
-      <c r="T55" s="6">
+      <c r="T55" s="8">
         <v>1444.74</v>
       </c>
       <c r="U55" s="5">
@@ -4830,7 +4836,7 @@
       <c r="S56" s="3">
         <v>2</v>
       </c>
-      <c r="T56" s="6">
+      <c r="T56" s="8">
         <v>1275.9000000000001</v>
       </c>
       <c r="U56" s="5">
@@ -4907,7 +4913,7 @@
       <c r="S57" s="3">
         <v>1</v>
       </c>
-      <c r="T57" s="3">
+      <c r="T57" s="8">
         <v>572.87</v>
       </c>
       <c r="U57" s="5">
@@ -4984,7 +4990,7 @@
       <c r="S58" s="3">
         <v>1</v>
       </c>
-      <c r="T58" s="3">
+      <c r="T58" s="8">
         <v>324.10000000000002</v>
       </c>
       <c r="U58" s="5">
@@ -5061,7 +5067,7 @@
       <c r="S59" s="3">
         <v>2</v>
       </c>
-      <c r="T59" s="3">
+      <c r="T59" s="8">
         <v>306.10000000000002</v>
       </c>
       <c r="U59" s="5">
@@ -5138,7 +5144,7 @@
       <c r="S60" s="3">
         <v>1</v>
       </c>
-      <c r="T60" s="3">
+      <c r="T60" s="8">
         <v>153.6</v>
       </c>
       <c r="U60" s="5">
@@ -5215,7 +5221,7 @@
       <c r="S61" s="3">
         <v>1</v>
       </c>
-      <c r="T61" s="3">
+      <c r="T61" s="8">
         <v>331.83</v>
       </c>
       <c r="U61" s="5">
@@ -5292,7 +5298,7 @@
       <c r="S62" s="3">
         <v>1</v>
       </c>
-      <c r="T62" s="3">
+      <c r="T62" s="8">
         <v>501</v>
       </c>
       <c r="U62" s="5">
@@ -5369,7 +5375,7 @@
       <c r="S63" s="3">
         <v>1</v>
       </c>
-      <c r="T63" s="3">
+      <c r="T63" s="8">
         <v>623.29999999999995</v>
       </c>
       <c r="U63" s="5">
@@ -5446,7 +5452,7 @@
       <c r="S64" s="3">
         <v>2</v>
       </c>
-      <c r="T64" s="3">
+      <c r="T64" s="8">
         <v>287.7</v>
       </c>
       <c r="U64" s="5">
@@ -5523,7 +5529,7 @@
       <c r="S65" s="3">
         <v>1</v>
       </c>
-      <c r="T65" s="3">
+      <c r="T65" s="8">
         <v>22.9</v>
       </c>
       <c r="U65" s="5">
@@ -5600,7 +5606,7 @@
       <c r="S66" s="3">
         <v>0</v>
       </c>
-      <c r="T66" s="3">
+      <c r="T66" s="8">
         <v>0</v>
       </c>
       <c r="U66" s="5">
@@ -5677,7 +5683,7 @@
       <c r="S67" s="3">
         <v>0</v>
       </c>
-      <c r="T67" s="3">
+      <c r="T67" s="8">
         <v>0</v>
       </c>
       <c r="U67" s="5">
@@ -5754,7 +5760,7 @@
       <c r="S68" s="3">
         <v>0</v>
       </c>
-      <c r="T68" s="3">
+      <c r="T68" s="8">
         <v>0</v>
       </c>
       <c r="U68" s="5">
@@ -5831,7 +5837,7 @@
       <c r="S69" s="3">
         <v>0</v>
       </c>
-      <c r="T69" s="3">
+      <c r="T69" s="8">
         <v>0</v>
       </c>
       <c r="U69" s="5">
@@ -5908,7 +5914,7 @@
       <c r="S70" s="3">
         <v>0</v>
       </c>
-      <c r="T70" s="3">
+      <c r="T70" s="8">
         <v>0</v>
       </c>
       <c r="U70" s="5">
@@ -5985,7 +5991,7 @@
       <c r="S71" s="3">
         <v>0</v>
       </c>
-      <c r="T71" s="3">
+      <c r="T71" s="8">
         <v>0</v>
       </c>
       <c r="U71" s="5">
@@ -6062,7 +6068,7 @@
       <c r="S72" s="3">
         <v>2</v>
       </c>
-      <c r="T72" s="6">
+      <c r="T72" s="8">
         <v>2256.1</v>
       </c>
       <c r="U72" s="5">
@@ -6139,7 +6145,7 @@
       <c r="S73" s="3">
         <v>1</v>
       </c>
-      <c r="T73" s="6">
+      <c r="T73" s="8">
         <v>1802.29</v>
       </c>
       <c r="U73" s="5">
@@ -6216,7 +6222,7 @@
       <c r="S74" s="3">
         <v>1</v>
       </c>
-      <c r="T74" s="3">
+      <c r="T74" s="8">
         <v>255.2</v>
       </c>
       <c r="U74" s="5">
@@ -6293,7 +6299,7 @@
       <c r="S75" s="3">
         <v>1</v>
       </c>
-      <c r="T75" s="6">
+      <c r="T75" s="8">
         <v>1086.8</v>
       </c>
       <c r="U75" s="5">
@@ -6370,7 +6376,7 @@
       <c r="S76" s="3">
         <v>1</v>
       </c>
-      <c r="T76" s="3">
+      <c r="T76" s="8">
         <v>340.5</v>
       </c>
       <c r="U76" s="5">
@@ -6447,7 +6453,7 @@
       <c r="S77" s="3">
         <v>1</v>
       </c>
-      <c r="T77" s="3">
+      <c r="T77" s="8">
         <v>554.66999999999996</v>
       </c>
       <c r="U77" s="5">
@@ -6524,7 +6530,7 @@
       <c r="S78" s="3">
         <v>1</v>
       </c>
-      <c r="T78" s="3">
+      <c r="T78" s="8">
         <v>264.5</v>
       </c>
       <c r="U78" s="5">
@@ -6601,7 +6607,7 @@
       <c r="S79" s="3">
         <v>1</v>
       </c>
-      <c r="T79" s="3">
+      <c r="T79" s="8">
         <v>296.10000000000002</v>
       </c>
       <c r="U79" s="5">
@@ -6678,7 +6684,7 @@
       <c r="S80" s="3">
         <v>1</v>
       </c>
-      <c r="T80" s="3">
+      <c r="T80" s="8">
         <v>500.26</v>
       </c>
       <c r="U80" s="5">
@@ -6755,7 +6761,7 @@
       <c r="S81" s="3">
         <v>1</v>
       </c>
-      <c r="T81" s="3">
+      <c r="T81" s="8">
         <v>268.3</v>
       </c>
       <c r="U81" s="5">
@@ -6832,7 +6838,7 @@
       <c r="S82" s="3">
         <v>1</v>
       </c>
-      <c r="T82" s="3">
+      <c r="T82" s="8">
         <v>521.66999999999996</v>
       </c>
       <c r="U82" s="5">
@@ -6909,7 +6915,7 @@
       <c r="S83" s="3">
         <v>1</v>
       </c>
-      <c r="T83" s="3">
+      <c r="T83" s="8">
         <v>344.5</v>
       </c>
       <c r="U83" s="5">
@@ -6986,7 +6992,7 @@
       <c r="S84" s="3">
         <v>1</v>
       </c>
-      <c r="T84" s="3">
+      <c r="T84" s="8">
         <v>171.6</v>
       </c>
       <c r="U84" s="5">
@@ -7063,7 +7069,7 @@
       <c r="S85" s="3">
         <v>1</v>
       </c>
-      <c r="T85" s="3">
+      <c r="T85" s="8">
         <v>503.52</v>
       </c>
       <c r="U85" s="5">
@@ -7140,7 +7146,7 @@
       <c r="S86" s="3">
         <v>1</v>
       </c>
-      <c r="T86" s="3">
+      <c r="T86" s="8">
         <v>720.53</v>
       </c>
       <c r="U86" s="5">
@@ -7217,7 +7223,7 @@
       <c r="S87" s="3">
         <v>1</v>
       </c>
-      <c r="T87" s="3">
+      <c r="T87" s="8">
         <v>372.86</v>
       </c>
       <c r="U87" s="5">
@@ -7294,7 +7300,7 @@
       <c r="S88" s="3">
         <v>1</v>
       </c>
-      <c r="T88" s="3">
+      <c r="T88" s="8">
         <v>626.54999999999995</v>
       </c>
       <c r="U88" s="5">
@@ -7371,7 +7377,7 @@
       <c r="S89" s="3">
         <v>1</v>
       </c>
-      <c r="T89" s="3">
+      <c r="T89" s="8">
         <v>145.6</v>
       </c>
       <c r="U89" s="5">
@@ -7448,7 +7454,7 @@
       <c r="S90" s="3">
         <v>1</v>
       </c>
-      <c r="T90" s="3">
+      <c r="T90" s="8">
         <v>458.19</v>
       </c>
       <c r="U90" s="5">
@@ -7525,7 +7531,7 @@
       <c r="S91" s="3">
         <v>1</v>
       </c>
-      <c r="T91" s="3">
+      <c r="T91" s="8">
         <v>218.9</v>
       </c>
       <c r="U91" s="5">
@@ -7602,7 +7608,7 @@
       <c r="S92" s="3">
         <v>1</v>
       </c>
-      <c r="T92" s="3">
+      <c r="T92" s="8">
         <v>63.8</v>
       </c>
       <c r="U92" s="5">
@@ -7679,7 +7685,7 @@
       <c r="S93" s="3">
         <v>1</v>
       </c>
-      <c r="T93" s="3">
+      <c r="T93" s="8">
         <v>224.5</v>
       </c>
       <c r="U93" s="5">
@@ -7756,7 +7762,7 @@
       <c r="S94" s="3">
         <v>1</v>
       </c>
-      <c r="T94" s="3">
+      <c r="T94" s="8">
         <v>180.3</v>
       </c>
       <c r="U94" s="5">
@@ -7833,7 +7839,7 @@
       <c r="S95" s="3">
         <v>1</v>
       </c>
-      <c r="T95" s="3">
+      <c r="T95" s="8">
         <v>449.9</v>
       </c>
       <c r="U95" s="5">
@@ -7910,7 +7916,7 @@
       <c r="S96" s="3">
         <v>1</v>
       </c>
-      <c r="T96" s="3">
+      <c r="T96" s="8">
         <v>135.75</v>
       </c>
       <c r="U96" s="5">
@@ -7987,7 +7993,7 @@
       <c r="S97" s="3">
         <v>1</v>
       </c>
-      <c r="T97" s="3">
+      <c r="T97" s="8">
         <v>197.55</v>
       </c>
       <c r="U97" s="5">
@@ -8064,7 +8070,7 @@
       <c r="S98" s="3">
         <v>1</v>
       </c>
-      <c r="T98" s="3">
+      <c r="T98" s="8">
         <v>166.7</v>
       </c>
       <c r="U98" s="5">
@@ -8141,7 +8147,7 @@
       <c r="S99" s="3">
         <v>1</v>
       </c>
-      <c r="T99" s="3">
+      <c r="T99" s="8">
         <v>199.6</v>
       </c>
       <c r="U99" s="5">
@@ -8218,7 +8224,7 @@
       <c r="S100" s="3">
         <v>1</v>
       </c>
-      <c r="T100" s="3">
+      <c r="T100" s="8">
         <v>295.33</v>
       </c>
       <c r="U100" s="5">
@@ -8295,7 +8301,7 @@
       <c r="S101" s="3">
         <v>1</v>
       </c>
-      <c r="T101" s="3">
+      <c r="T101" s="8">
         <v>539.86</v>
       </c>
       <c r="U101" s="5">
@@ -8372,7 +8378,7 @@
       <c r="S102" s="3">
         <v>1</v>
       </c>
-      <c r="T102" s="3">
+      <c r="T102" s="8">
         <v>114.9</v>
       </c>
       <c r="U102" s="5">
@@ -8449,7 +8455,7 @@
       <c r="S103" s="3">
         <v>1</v>
       </c>
-      <c r="T103" s="3">
+      <c r="T103" s="8">
         <v>76.900000000000006</v>
       </c>
       <c r="U103" s="5">
@@ -8526,7 +8532,7 @@
       <c r="S104" s="3">
         <v>1</v>
       </c>
-      <c r="T104" s="3">
+      <c r="T104" s="8">
         <v>106.79</v>
       </c>
       <c r="U104" s="5">
@@ -8603,7 +8609,7 @@
       <c r="S105" s="3">
         <v>1</v>
       </c>
-      <c r="T105" s="3">
+      <c r="T105" s="8">
         <v>130.9</v>
       </c>
       <c r="U105" s="5">
@@ -8680,7 +8686,7 @@
       <c r="S106" s="3">
         <v>1</v>
       </c>
-      <c r="T106" s="3">
+      <c r="T106" s="8">
         <v>40.9</v>
       </c>
       <c r="U106" s="5">
@@ -8757,7 +8763,7 @@
       <c r="S107" s="3">
         <v>1</v>
       </c>
-      <c r="T107" s="3">
+      <c r="T107" s="8">
         <v>629.39</v>
       </c>
       <c r="U107" s="5">
@@ -8834,7 +8840,7 @@
       <c r="S108" s="3">
         <v>1</v>
       </c>
-      <c r="T108" s="3">
+      <c r="T108" s="8">
         <v>128.82</v>
       </c>
       <c r="U108" s="5">
@@ -8911,7 +8917,7 @@
       <c r="S109" s="3">
         <v>1</v>
       </c>
-      <c r="T109" s="3">
+      <c r="T109" s="8">
         <v>171.8</v>
       </c>
       <c r="U109" s="5">
@@ -8988,7 +8994,7 @@
       <c r="S110" s="3">
         <v>1</v>
       </c>
-      <c r="T110" s="3">
+      <c r="T110" s="8">
         <v>144</v>
       </c>
       <c r="U110" s="5">
@@ -9065,7 +9071,7 @@
       <c r="S111" s="3">
         <v>1</v>
       </c>
-      <c r="T111" s="3">
+      <c r="T111" s="8">
         <v>130.30000000000001</v>
       </c>
       <c r="U111" s="5">
@@ -9142,7 +9148,7 @@
       <c r="S112" s="3">
         <v>1</v>
       </c>
-      <c r="T112" s="3">
+      <c r="T112" s="8">
         <v>112.9</v>
       </c>
       <c r="U112" s="5">
@@ -9219,7 +9225,7 @@
       <c r="S113" s="3">
         <v>1</v>
       </c>
-      <c r="T113" s="3">
+      <c r="T113" s="8">
         <v>144</v>
       </c>
       <c r="U113" s="5">
@@ -9296,7 +9302,7 @@
       <c r="S114" s="3">
         <v>1</v>
       </c>
-      <c r="T114" s="3">
+      <c r="T114" s="8">
         <v>45.8</v>
       </c>
       <c r="U114" s="5">
@@ -9373,7 +9379,7 @@
       <c r="S115" s="3">
         <v>1</v>
       </c>
-      <c r="T115" s="3">
+      <c r="T115" s="8">
         <v>158.69999999999999</v>
       </c>
       <c r="U115" s="5">
@@ -9450,7 +9456,7 @@
       <c r="S116" s="3">
         <v>1</v>
       </c>
-      <c r="T116" s="3">
+      <c r="T116" s="8">
         <v>854.55</v>
       </c>
       <c r="U116" s="5">
@@ -9527,7 +9533,7 @@
       <c r="S117" s="3">
         <v>1</v>
       </c>
-      <c r="T117" s="3">
+      <c r="T117" s="8">
         <v>171.8</v>
       </c>
       <c r="U117" s="5">
@@ -9604,7 +9610,7 @@
       <c r="S118" s="3">
         <v>1</v>
       </c>
-      <c r="T118" s="3">
+      <c r="T118" s="8">
         <v>758.45</v>
       </c>
       <c r="U118" s="5">
@@ -9681,7 +9687,7 @@
       <c r="S119" s="3">
         <v>1</v>
       </c>
-      <c r="T119" s="3">
+      <c r="T119" s="8">
         <v>111.05</v>
       </c>
       <c r="U119" s="5">
@@ -9758,7 +9764,7 @@
       <c r="S120" s="3">
         <v>1</v>
       </c>
-      <c r="T120" s="3">
+      <c r="T120" s="8">
         <v>247.23</v>
       </c>
       <c r="U120" s="5">
@@ -9835,7 +9841,7 @@
       <c r="S121" s="3">
         <v>1</v>
       </c>
-      <c r="T121" s="3">
+      <c r="T121" s="8">
         <v>359.27</v>
       </c>
       <c r="U121" s="5">
@@ -9912,7 +9918,7 @@
       <c r="S122" s="3">
         <v>1</v>
       </c>
-      <c r="T122" s="3">
+      <c r="T122" s="8">
         <v>51.4</v>
       </c>
       <c r="U122" s="5">
@@ -9989,7 +9995,7 @@
       <c r="S123" s="3">
         <v>1</v>
       </c>
-      <c r="T123" s="3">
+      <c r="T123" s="8">
         <v>630.76</v>
       </c>
       <c r="U123" s="5">
@@ -10066,7 +10072,7 @@
       <c r="S124" s="3">
         <v>1</v>
       </c>
-      <c r="T124" s="3">
+      <c r="T124" s="8">
         <v>163.57</v>
       </c>
       <c r="U124" s="5">
@@ -10143,7 +10149,7 @@
       <c r="S125" s="3">
         <v>1</v>
       </c>
-      <c r="T125" s="3">
+      <c r="T125" s="8">
         <v>372.52</v>
       </c>
       <c r="U125" s="5">
@@ -10220,7 +10226,7 @@
       <c r="S126" s="3">
         <v>1</v>
       </c>
-      <c r="T126" s="3">
+      <c r="T126" s="8">
         <v>372.5</v>
       </c>
       <c r="U126" s="5">
@@ -10297,7 +10303,7 @@
       <c r="S127" s="3">
         <v>1</v>
       </c>
-      <c r="T127" s="3">
+      <c r="T127" s="8">
         <v>271.39</v>
       </c>
       <c r="U127" s="5">
@@ -10374,7 +10380,7 @@
       <c r="S128" s="3">
         <v>1</v>
       </c>
-      <c r="T128" s="3">
+      <c r="T128" s="8">
         <v>118.57</v>
       </c>
       <c r="U128" s="5">
@@ -10451,7 +10457,7 @@
       <c r="S129" s="3">
         <v>1</v>
       </c>
-      <c r="T129" s="3">
+      <c r="T129" s="8">
         <v>340.7</v>
       </c>
       <c r="U129" s="5">
@@ -10528,7 +10534,7 @@
       <c r="S130" s="3">
         <v>1</v>
       </c>
-      <c r="T130" s="3">
+      <c r="T130" s="8">
         <v>104.7</v>
       </c>
       <c r="U130" s="5">
@@ -10605,7 +10611,7 @@
       <c r="S131" s="3">
         <v>1</v>
       </c>
-      <c r="T131" s="3">
+      <c r="T131" s="8">
         <v>377.18</v>
       </c>
       <c r="U131" s="5">
@@ -10682,7 +10688,7 @@
       <c r="S132" s="3">
         <v>1</v>
       </c>
-      <c r="T132" s="3">
+      <c r="T132" s="8">
         <v>227.36</v>
       </c>
       <c r="U132" s="5">
@@ -10759,7 +10765,7 @@
       <c r="S133" s="3">
         <v>1</v>
       </c>
-      <c r="T133" s="3">
+      <c r="T133" s="8">
         <v>530.83000000000004</v>
       </c>
       <c r="U133" s="5">
@@ -10836,7 +10842,7 @@
       <c r="S134" s="3">
         <v>1</v>
       </c>
-      <c r="T134" s="3">
+      <c r="T134" s="8">
         <v>104.21</v>
       </c>
       <c r="U134" s="5">
@@ -10913,7 +10919,7 @@
       <c r="S135" s="3">
         <v>1</v>
       </c>
-      <c r="T135" s="3">
+      <c r="T135" s="8">
         <v>276.62</v>
       </c>
       <c r="U135" s="5">
@@ -10990,7 +10996,7 @@
       <c r="S136" s="3">
         <v>1</v>
       </c>
-      <c r="T136" s="3">
+      <c r="T136" s="8">
         <v>150.94</v>
       </c>
       <c r="U136" s="5">
@@ -11067,7 +11073,7 @@
       <c r="S137" s="3">
         <v>1</v>
       </c>
-      <c r="T137" s="3">
+      <c r="T137" s="8">
         <v>145.6</v>
       </c>
       <c r="U137" s="5">
@@ -11144,7 +11150,7 @@
       <c r="S138" s="3">
         <v>1</v>
       </c>
-      <c r="T138" s="6">
+      <c r="T138" s="8">
         <v>1680.87</v>
       </c>
       <c r="U138" s="5">
@@ -11221,7 +11227,7 @@
       <c r="S139" s="3">
         <v>1</v>
       </c>
-      <c r="T139" s="6">
+      <c r="T139" s="8">
         <v>3252.82</v>
       </c>
       <c r="U139" s="5">
@@ -11298,7 +11304,7 @@
       <c r="S140" s="3">
         <v>1</v>
       </c>
-      <c r="T140" s="3">
+      <c r="T140" s="8">
         <v>193.54</v>
       </c>
       <c r="U140" s="5">
@@ -11375,7 +11381,7 @@
       <c r="S141" s="3">
         <v>1</v>
       </c>
-      <c r="T141" s="3">
+      <c r="T141" s="8">
         <v>112.7</v>
       </c>
       <c r="U141" s="5">
@@ -11452,7 +11458,7 @@
       <c r="S142" s="3">
         <v>1</v>
       </c>
-      <c r="T142" s="3">
+      <c r="T142" s="8">
         <v>63.77</v>
       </c>
       <c r="U142" s="5">
@@ -11529,7 +11535,7 @@
       <c r="S143" s="3">
         <v>1</v>
       </c>
-      <c r="T143" s="3">
+      <c r="T143" s="8">
         <v>217.13</v>
       </c>
       <c r="U143" s="5">
@@ -11606,7 +11612,7 @@
       <c r="S144" s="3">
         <v>1</v>
       </c>
-      <c r="T144" s="6">
+      <c r="T144" s="8">
         <v>1274.22</v>
       </c>
       <c r="U144" s="5">
@@ -11683,7 +11689,7 @@
       <c r="S145" s="3">
         <v>1</v>
       </c>
-      <c r="T145" s="3">
+      <c r="T145" s="8">
         <v>695.25</v>
       </c>
       <c r="U145" s="5">
@@ -11760,7 +11766,7 @@
       <c r="S146" s="3">
         <v>1</v>
       </c>
-      <c r="T146" s="3">
+      <c r="T146" s="8">
         <v>952.79</v>
       </c>
       <c r="U146" s="5">
@@ -11837,7 +11843,7 @@
       <c r="S147" s="3">
         <v>1</v>
       </c>
-      <c r="T147" s="3">
+      <c r="T147" s="8">
         <v>794.69</v>
       </c>
       <c r="U147" s="5">
@@ -11914,7 +11920,7 @@
       <c r="S148" s="3">
         <v>1</v>
       </c>
-      <c r="T148" s="3">
+      <c r="T148" s="8">
         <v>965.29</v>
       </c>
       <c r="U148" s="5">
@@ -11991,7 +11997,7 @@
       <c r="S149" s="3">
         <v>1</v>
       </c>
-      <c r="T149" s="6">
+      <c r="T149" s="8">
         <v>3246.27</v>
       </c>
       <c r="U149" s="5">
@@ -12068,7 +12074,7 @@
       <c r="S150" s="3">
         <v>1</v>
       </c>
-      <c r="T150" s="6">
+      <c r="T150" s="8">
         <v>1305.3</v>
       </c>
       <c r="U150" s="5">
@@ -12145,7 +12151,7 @@
       <c r="S151" s="3">
         <v>1</v>
       </c>
-      <c r="T151" s="3">
+      <c r="T151" s="8">
         <v>502.69</v>
       </c>
       <c r="U151" s="5">
@@ -12222,7 +12228,7 @@
       <c r="S152" s="3">
         <v>1</v>
       </c>
-      <c r="T152" s="3">
+      <c r="T152" s="8">
         <v>629.91999999999996</v>
       </c>
       <c r="U152" s="5">
@@ -12299,7 +12305,7 @@
       <c r="S153" s="3">
         <v>1</v>
       </c>
-      <c r="T153" s="3">
+      <c r="T153" s="8">
         <v>433.53</v>
       </c>
       <c r="U153" s="5">
@@ -12376,7 +12382,7 @@
       <c r="S154" s="3">
         <v>1</v>
       </c>
-      <c r="T154" s="3">
+      <c r="T154" s="8">
         <v>155.72</v>
       </c>
       <c r="U154" s="5">
@@ -12399,61 +12405,61 @@
       <c r="A155" s="4">
         <v>45200</v>
       </c>
-      <c r="B155" s="7">
+      <c r="B155" s="3">
         <v>74</v>
       </c>
-      <c r="C155" s="7">
+      <c r="C155" s="3">
         <v>131</v>
       </c>
-      <c r="D155" s="7">
-        <v>3</v>
-      </c>
-      <c r="E155" s="7">
+      <c r="D155" s="3">
+        <v>3</v>
+      </c>
+      <c r="E155" s="3">
         <v>22</v>
       </c>
       <c r="F155" s="5">
         <v>0.29730000000000001</v>
       </c>
-      <c r="G155" s="7">
+      <c r="G155" s="3">
         <v>18</v>
       </c>
-      <c r="H155" s="7">
+      <c r="H155" s="3">
         <v>2</v>
       </c>
-      <c r="I155" s="7">
+      <c r="I155" s="3">
         <v>9</v>
       </c>
-      <c r="J155" s="7">
+      <c r="J155" s="3">
         <v>8</v>
       </c>
       <c r="K155" s="5">
         <v>0.1216</v>
       </c>
-      <c r="L155" s="7">
-        <v>3</v>
-      </c>
-      <c r="M155" s="7">
+      <c r="L155" s="3">
+        <v>3</v>
+      </c>
+      <c r="M155" s="3">
         <v>5</v>
       </c>
-      <c r="N155" s="7">
-        <v>1</v>
-      </c>
-      <c r="O155" s="7">
+      <c r="N155" s="3">
+        <v>1</v>
+      </c>
+      <c r="O155" s="3">
         <v>104.64</v>
       </c>
       <c r="P155" s="5">
         <v>4.0500000000000001E-2</v>
       </c>
-      <c r="Q155" s="7">
-        <v>3</v>
-      </c>
-      <c r="R155" s="7">
+      <c r="Q155" s="3">
+        <v>3</v>
+      </c>
+      <c r="R155" s="3">
         <v>5</v>
       </c>
-      <c r="S155" s="7">
-        <v>1</v>
-      </c>
-      <c r="T155" s="7">
+      <c r="S155" s="3">
+        <v>1</v>
+      </c>
+      <c r="T155" s="8">
         <v>104.64</v>
       </c>
       <c r="U155" s="5">
@@ -12476,61 +12482,61 @@
       <c r="A156" s="4">
         <v>45201</v>
       </c>
-      <c r="B156" s="7">
+      <c r="B156" s="3">
         <v>129</v>
       </c>
-      <c r="C156" s="7">
+      <c r="C156" s="3">
         <v>275</v>
       </c>
-      <c r="D156" s="7">
-        <v>3</v>
-      </c>
-      <c r="E156" s="7">
+      <c r="D156" s="3">
+        <v>3</v>
+      </c>
+      <c r="E156" s="3">
         <v>29</v>
       </c>
       <c r="F156" s="5">
         <v>0.2248</v>
       </c>
-      <c r="G156" s="7">
+      <c r="G156" s="3">
         <v>31</v>
       </c>
-      <c r="H156" s="7">
-        <v>1</v>
-      </c>
-      <c r="I156" s="7">
+      <c r="H156" s="3">
+        <v>1</v>
+      </c>
+      <c r="I156" s="3">
         <v>81</v>
       </c>
-      <c r="J156" s="7">
+      <c r="J156" s="3">
         <v>162</v>
       </c>
       <c r="K156" s="5">
         <v>0.62790000000000001</v>
       </c>
-      <c r="L156" s="7">
+      <c r="L156" s="3">
         <v>35</v>
       </c>
-      <c r="M156" s="7">
+      <c r="M156" s="3">
         <v>45</v>
       </c>
-      <c r="N156" s="7">
-        <v>1</v>
-      </c>
-      <c r="O156" s="7">
+      <c r="N156" s="3">
+        <v>1</v>
+      </c>
+      <c r="O156" s="3">
         <v>863.24</v>
       </c>
       <c r="P156" s="5">
         <v>0.27129999999999999</v>
       </c>
-      <c r="Q156" s="7">
+      <c r="Q156" s="3">
         <v>32</v>
       </c>
-      <c r="R156" s="7">
+      <c r="R156" s="3">
         <v>38</v>
       </c>
-      <c r="S156" s="7">
-        <v>1</v>
-      </c>
-      <c r="T156" s="7">
+      <c r="S156" s="3">
+        <v>1</v>
+      </c>
+      <c r="T156" s="8">
         <v>748.49</v>
       </c>
       <c r="U156" s="5">
@@ -12553,61 +12559,61 @@
       <c r="A157" s="4">
         <v>45202</v>
       </c>
-      <c r="B157" s="7">
+      <c r="B157" s="3">
         <v>96</v>
       </c>
-      <c r="C157" s="7">
+      <c r="C157" s="3">
         <v>162</v>
       </c>
-      <c r="D157" s="7">
-        <v>3</v>
-      </c>
-      <c r="E157" s="7">
+      <c r="D157" s="3">
+        <v>3</v>
+      </c>
+      <c r="E157" s="3">
         <v>21</v>
       </c>
       <c r="F157" s="5">
         <v>0.21879999999999999</v>
       </c>
-      <c r="G157" s="7">
+      <c r="G157" s="3">
         <v>35</v>
       </c>
-      <c r="H157" s="7">
+      <c r="H157" s="3">
         <v>2</v>
       </c>
-      <c r="I157" s="7">
+      <c r="I157" s="3">
         <v>43</v>
       </c>
-      <c r="J157" s="7">
+      <c r="J157" s="3">
         <v>72</v>
       </c>
       <c r="K157" s="5">
         <v>0.44790000000000002</v>
       </c>
-      <c r="L157" s="7">
+      <c r="L157" s="3">
         <v>19</v>
       </c>
-      <c r="M157" s="7">
+      <c r="M157" s="3">
         <v>19</v>
       </c>
-      <c r="N157" s="7">
-        <v>1</v>
-      </c>
-      <c r="O157" s="7">
+      <c r="N157" s="3">
+        <v>1</v>
+      </c>
+      <c r="O157" s="3">
         <v>458.32</v>
       </c>
       <c r="P157" s="5">
         <v>0.19789999999999999</v>
       </c>
-      <c r="Q157" s="7">
+      <c r="Q157" s="3">
         <v>19</v>
       </c>
-      <c r="R157" s="7">
+      <c r="R157" s="3">
         <v>19</v>
       </c>
-      <c r="S157" s="7">
-        <v>1</v>
-      </c>
-      <c r="T157" s="7">
+      <c r="S157" s="3">
+        <v>1</v>
+      </c>
+      <c r="T157" s="8">
         <v>458.32</v>
       </c>
       <c r="U157" s="5">
@@ -12630,61 +12636,61 @@
       <c r="A158" s="4">
         <v>45203</v>
       </c>
-      <c r="B158" s="7">
+      <c r="B158" s="3">
         <v>111</v>
       </c>
-      <c r="C158" s="7">
+      <c r="C158" s="3">
         <v>183</v>
       </c>
-      <c r="D158" s="7">
-        <v>3</v>
-      </c>
-      <c r="E158" s="7">
+      <c r="D158" s="3">
+        <v>3</v>
+      </c>
+      <c r="E158" s="3">
         <v>22</v>
       </c>
       <c r="F158" s="5">
         <v>0.19819999999999999</v>
       </c>
-      <c r="G158" s="7">
+      <c r="G158" s="3">
         <v>21</v>
       </c>
-      <c r="H158" s="7">
-        <v>0</v>
-      </c>
-      <c r="I158" s="7">
+      <c r="H158" s="3">
+        <v>0</v>
+      </c>
+      <c r="I158" s="3">
         <v>78</v>
       </c>
-      <c r="J158" s="7">
+      <c r="J158" s="3">
         <v>116</v>
       </c>
       <c r="K158" s="5">
         <v>0.70269999999999999</v>
       </c>
-      <c r="L158" s="7">
+      <c r="L158" s="3">
         <v>11</v>
       </c>
-      <c r="M158" s="7">
+      <c r="M158" s="3">
         <v>11</v>
       </c>
-      <c r="N158" s="7">
-        <v>1</v>
-      </c>
-      <c r="O158" s="7">
+      <c r="N158" s="3">
+        <v>1</v>
+      </c>
+      <c r="O158" s="3">
         <v>315.64999999999998</v>
       </c>
       <c r="P158" s="5">
         <v>9.9099999999999994E-2</v>
       </c>
-      <c r="Q158" s="7">
+      <c r="Q158" s="3">
         <v>9</v>
       </c>
-      <c r="R158" s="7">
+      <c r="R158" s="3">
         <v>9</v>
       </c>
-      <c r="S158" s="7">
-        <v>1</v>
-      </c>
-      <c r="T158" s="7">
+      <c r="S158" s="3">
+        <v>1</v>
+      </c>
+      <c r="T158" s="8">
         <v>243.85</v>
       </c>
       <c r="U158" s="5">
@@ -12707,61 +12713,61 @@
       <c r="A159" s="4">
         <v>45204</v>
       </c>
-      <c r="B159" s="7">
+      <c r="B159" s="3">
         <v>74</v>
       </c>
-      <c r="C159" s="7">
+      <c r="C159" s="3">
         <v>143</v>
       </c>
-      <c r="D159" s="7">
-        <v>1</v>
-      </c>
-      <c r="E159" s="7">
+      <c r="D159" s="3">
+        <v>1</v>
+      </c>
+      <c r="E159" s="3">
         <v>15</v>
       </c>
       <c r="F159" s="5">
         <v>0.20269999999999999</v>
       </c>
-      <c r="G159" s="7">
+      <c r="G159" s="3">
         <v>17</v>
       </c>
-      <c r="H159" s="7">
-        <v>1</v>
-      </c>
-      <c r="I159" s="7">
+      <c r="H159" s="3">
+        <v>1</v>
+      </c>
+      <c r="I159" s="3">
         <v>48</v>
       </c>
-      <c r="J159" s="7">
+      <c r="J159" s="3">
         <v>90</v>
       </c>
       <c r="K159" s="5">
         <v>0.64859999999999995</v>
       </c>
-      <c r="L159" s="7">
+      <c r="L159" s="3">
         <v>17</v>
       </c>
-      <c r="M159" s="7">
+      <c r="M159" s="3">
         <v>21</v>
       </c>
-      <c r="N159" s="7">
-        <v>1</v>
-      </c>
-      <c r="O159" s="7">
+      <c r="N159" s="3">
+        <v>1</v>
+      </c>
+      <c r="O159" s="3">
         <v>329.38</v>
       </c>
       <c r="P159" s="5">
         <v>0.22969999999999999</v>
       </c>
-      <c r="Q159" s="7">
+      <c r="Q159" s="3">
         <v>15</v>
       </c>
-      <c r="R159" s="7">
+      <c r="R159" s="3">
         <v>16</v>
       </c>
-      <c r="S159" s="7">
-        <v>1</v>
-      </c>
-      <c r="T159" s="7">
+      <c r="S159" s="3">
+        <v>1</v>
+      </c>
+      <c r="T159" s="8">
         <v>267.98</v>
       </c>
       <c r="U159" s="5">
@@ -12784,61 +12790,61 @@
       <c r="A160" s="4">
         <v>45205</v>
       </c>
-      <c r="B160" s="7">
+      <c r="B160" s="3">
         <v>52</v>
       </c>
-      <c r="C160" s="7">
+      <c r="C160" s="3">
         <v>103</v>
       </c>
-      <c r="D160" s="7">
-        <v>3</v>
-      </c>
-      <c r="E160" s="7">
+      <c r="D160" s="3">
+        <v>3</v>
+      </c>
+      <c r="E160" s="3">
         <v>9</v>
       </c>
       <c r="F160" s="5">
         <v>0.1731</v>
       </c>
-      <c r="G160" s="7">
+      <c r="G160" s="3">
         <v>17</v>
       </c>
-      <c r="H160" s="7">
-        <v>1</v>
-      </c>
-      <c r="I160" s="7">
+      <c r="H160" s="3">
+        <v>1</v>
+      </c>
+      <c r="I160" s="3">
         <v>20</v>
       </c>
-      <c r="J160" s="7">
+      <c r="J160" s="3">
         <v>27</v>
       </c>
       <c r="K160" s="5">
         <v>0.3846</v>
       </c>
-      <c r="L160" s="7">
+      <c r="L160" s="3">
         <v>5</v>
       </c>
-      <c r="M160" s="7">
+      <c r="M160" s="3">
         <v>8</v>
       </c>
-      <c r="N160" s="7">
-        <v>1</v>
-      </c>
-      <c r="O160" s="7">
+      <c r="N160" s="3">
+        <v>1</v>
+      </c>
+      <c r="O160" s="3">
         <v>137.79</v>
       </c>
       <c r="P160" s="5">
         <v>9.6199999999999994E-2</v>
       </c>
-      <c r="Q160" s="7">
+      <c r="Q160" s="3">
         <v>5</v>
       </c>
-      <c r="R160" s="7">
+      <c r="R160" s="3">
         <v>8</v>
       </c>
-      <c r="S160" s="7">
-        <v>1</v>
-      </c>
-      <c r="T160" s="7">
+      <c r="S160" s="3">
+        <v>1</v>
+      </c>
+      <c r="T160" s="8">
         <v>137.79</v>
       </c>
       <c r="U160" s="5">
@@ -12861,61 +12867,61 @@
       <c r="A161" s="4">
         <v>45206</v>
       </c>
-      <c r="B161" s="7">
+      <c r="B161" s="3">
         <v>32</v>
       </c>
-      <c r="C161" s="7">
+      <c r="C161" s="3">
         <v>56</v>
       </c>
-      <c r="D161" s="7">
-        <v>1</v>
-      </c>
-      <c r="E161" s="7">
+      <c r="D161" s="3">
+        <v>1</v>
+      </c>
+      <c r="E161" s="3">
         <v>5</v>
       </c>
       <c r="F161" s="5">
         <v>0.15620000000000001</v>
       </c>
-      <c r="G161" s="7">
+      <c r="G161" s="3">
         <v>9</v>
       </c>
-      <c r="H161" s="7">
-        <v>0</v>
-      </c>
-      <c r="I161" s="7">
+      <c r="H161" s="3">
+        <v>0</v>
+      </c>
+      <c r="I161" s="3">
         <v>9</v>
       </c>
-      <c r="J161" s="7">
+      <c r="J161" s="3">
         <v>8</v>
       </c>
       <c r="K161" s="5">
         <v>0.28120000000000001</v>
       </c>
-      <c r="L161" s="7">
-        <v>1</v>
-      </c>
-      <c r="M161" s="7">
-        <v>1</v>
-      </c>
-      <c r="N161" s="7">
-        <v>1</v>
-      </c>
-      <c r="O161" s="7">
+      <c r="L161" s="3">
+        <v>1</v>
+      </c>
+      <c r="M161" s="3">
+        <v>1</v>
+      </c>
+      <c r="N161" s="3">
+        <v>1</v>
+      </c>
+      <c r="O161" s="3">
         <v>22.9</v>
       </c>
       <c r="P161" s="5">
         <v>3.1199999999999999E-2</v>
       </c>
-      <c r="Q161" s="7">
-        <v>1</v>
-      </c>
-      <c r="R161" s="7">
-        <v>1</v>
-      </c>
-      <c r="S161" s="7">
-        <v>1</v>
-      </c>
-      <c r="T161" s="7">
+      <c r="Q161" s="3">
+        <v>1</v>
+      </c>
+      <c r="R161" s="3">
+        <v>1</v>
+      </c>
+      <c r="S161" s="3">
+        <v>1</v>
+      </c>
+      <c r="T161" s="8">
         <v>22.9</v>
       </c>
       <c r="U161" s="5">
@@ -12938,61 +12944,61 @@
       <c r="A162" s="4">
         <v>45207</v>
       </c>
-      <c r="B162" s="7">
+      <c r="B162" s="3">
         <v>39</v>
       </c>
-      <c r="C162" s="7">
+      <c r="C162" s="3">
         <v>79</v>
       </c>
-      <c r="D162" s="7">
-        <v>1</v>
-      </c>
-      <c r="E162" s="7">
+      <c r="D162" s="3">
+        <v>1</v>
+      </c>
+      <c r="E162" s="3">
         <v>8</v>
       </c>
       <c r="F162" s="5">
         <v>0.2051</v>
       </c>
-      <c r="G162" s="7">
+      <c r="G162" s="3">
         <v>16</v>
       </c>
-      <c r="H162" s="7">
-        <v>1</v>
-      </c>
-      <c r="I162" s="7">
+      <c r="H162" s="3">
+        <v>1</v>
+      </c>
+      <c r="I162" s="3">
         <v>5</v>
       </c>
-      <c r="J162" s="7">
+      <c r="J162" s="3">
         <v>8</v>
       </c>
       <c r="K162" s="5">
         <v>0.12820000000000001</v>
       </c>
-      <c r="L162" s="7">
-        <v>1</v>
-      </c>
-      <c r="M162" s="7">
-        <v>1</v>
-      </c>
-      <c r="N162" s="7">
-        <v>1</v>
-      </c>
-      <c r="O162" s="7">
+      <c r="L162" s="3">
+        <v>1</v>
+      </c>
+      <c r="M162" s="3">
+        <v>1</v>
+      </c>
+      <c r="N162" s="3">
+        <v>1</v>
+      </c>
+      <c r="O162" s="3">
         <v>38.28</v>
       </c>
       <c r="P162" s="5">
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="Q162" s="7">
-        <v>1</v>
-      </c>
-      <c r="R162" s="7">
-        <v>1</v>
-      </c>
-      <c r="S162" s="7">
-        <v>1</v>
-      </c>
-      <c r="T162" s="7">
+      <c r="Q162" s="3">
+        <v>1</v>
+      </c>
+      <c r="R162" s="3">
+        <v>1</v>
+      </c>
+      <c r="S162" s="3">
+        <v>1</v>
+      </c>
+      <c r="T162" s="8">
         <v>38.28</v>
       </c>
       <c r="U162" s="5">
@@ -13015,43 +13021,43 @@
       <c r="A163" s="4">
         <v>45208</v>
       </c>
-      <c r="B163" s="7">
+      <c r="B163" s="3">
         <v>160</v>
       </c>
-      <c r="C163" s="7">
+      <c r="C163" s="3">
         <v>374</v>
       </c>
-      <c r="D163" s="7">
-        <v>3</v>
-      </c>
-      <c r="E163" s="7">
+      <c r="D163" s="3">
+        <v>3</v>
+      </c>
+      <c r="E163" s="3">
         <v>33</v>
       </c>
       <c r="F163" s="5">
         <v>0.20619999999999999</v>
       </c>
-      <c r="G163" s="7">
+      <c r="G163" s="3">
         <v>35</v>
       </c>
-      <c r="H163" s="7">
-        <v>1</v>
-      </c>
-      <c r="I163" s="7">
+      <c r="H163" s="3">
+        <v>1</v>
+      </c>
+      <c r="I163" s="3">
         <v>125</v>
       </c>
-      <c r="J163" s="7">
+      <c r="J163" s="3">
         <v>217</v>
       </c>
       <c r="K163" s="5">
         <v>0.78120000000000001</v>
       </c>
-      <c r="L163" s="7">
+      <c r="L163" s="3">
         <v>53</v>
       </c>
-      <c r="M163" s="7">
+      <c r="M163" s="3">
         <v>63</v>
       </c>
-      <c r="N163" s="7">
+      <c r="N163" s="3">
         <v>1</v>
       </c>
       <c r="O163" s="6">
@@ -13060,16 +13066,16 @@
       <c r="P163" s="5">
         <v>0.33119999999999999</v>
       </c>
-      <c r="Q163" s="7">
+      <c r="Q163" s="3">
         <v>51</v>
       </c>
-      <c r="R163" s="7">
+      <c r="R163" s="3">
         <v>57</v>
       </c>
-      <c r="S163" s="7">
-        <v>1</v>
-      </c>
-      <c r="T163" s="6">
+      <c r="S163" s="3">
+        <v>1</v>
+      </c>
+      <c r="T163" s="8">
         <v>1014</v>
       </c>
       <c r="U163" s="5">
@@ -13092,43 +13098,43 @@
       <c r="A164" s="4">
         <v>45209</v>
       </c>
-      <c r="B164" s="7">
+      <c r="B164" s="3">
         <v>507</v>
       </c>
-      <c r="C164" s="7">
+      <c r="C164" s="3">
         <v>1233</v>
       </c>
-      <c r="D164" s="7">
-        <v>3</v>
-      </c>
-      <c r="E164" s="7">
+      <c r="D164" s="3">
+        <v>3</v>
+      </c>
+      <c r="E164" s="3">
         <v>79</v>
       </c>
       <c r="F164" s="5">
         <v>0.15579999999999999</v>
       </c>
-      <c r="G164" s="7">
+      <c r="G164" s="3">
         <v>106</v>
       </c>
-      <c r="H164" s="7">
+      <c r="H164" s="3">
         <v>4</v>
       </c>
-      <c r="I164" s="7">
+      <c r="I164" s="3">
         <v>519</v>
       </c>
-      <c r="J164" s="7">
+      <c r="J164" s="3">
         <v>1115</v>
       </c>
       <c r="K164" s="5">
         <v>1.0237000000000001</v>
       </c>
-      <c r="L164" s="7">
+      <c r="L164" s="3">
         <v>199</v>
       </c>
-      <c r="M164" s="7">
+      <c r="M164" s="3">
         <v>217</v>
       </c>
-      <c r="N164" s="7">
+      <c r="N164" s="3">
         <v>2</v>
       </c>
       <c r="O164" s="6">
@@ -13137,16 +13143,16 @@
       <c r="P164" s="5">
         <v>0.39250000000000002</v>
       </c>
-      <c r="Q164" s="7">
+      <c r="Q164" s="3">
         <v>184</v>
       </c>
-      <c r="R164" s="7">
+      <c r="R164" s="3">
         <v>198</v>
       </c>
-      <c r="S164" s="7">
+      <c r="S164" s="3">
         <v>2</v>
       </c>
-      <c r="T164" s="6">
+      <c r="T164" s="8">
         <v>2732.79</v>
       </c>
       <c r="U164" s="5">
@@ -13169,43 +13175,43 @@
       <c r="A165" s="4">
         <v>45210</v>
       </c>
-      <c r="B165" s="7">
+      <c r="B165" s="3">
         <v>237</v>
       </c>
-      <c r="C165" s="7">
+      <c r="C165" s="3">
         <v>583</v>
       </c>
-      <c r="D165" s="7">
-        <v>3</v>
-      </c>
-      <c r="E165" s="7">
+      <c r="D165" s="3">
+        <v>3</v>
+      </c>
+      <c r="E165" s="3">
         <v>53</v>
       </c>
       <c r="F165" s="5">
         <v>0.22359999999999999</v>
       </c>
-      <c r="G165" s="7">
+      <c r="G165" s="3">
         <v>44</v>
       </c>
-      <c r="H165" s="7">
+      <c r="H165" s="3">
         <v>4</v>
       </c>
-      <c r="I165" s="7">
+      <c r="I165" s="3">
         <v>203</v>
       </c>
-      <c r="J165" s="7">
+      <c r="J165" s="3">
         <v>426</v>
       </c>
       <c r="K165" s="5">
         <v>0.85650000000000004</v>
       </c>
-      <c r="L165" s="7">
+      <c r="L165" s="3">
         <v>72</v>
       </c>
-      <c r="M165" s="7">
+      <c r="M165" s="3">
         <v>89</v>
       </c>
-      <c r="N165" s="7">
+      <c r="N165" s="3">
         <v>2</v>
       </c>
       <c r="O165" s="6">
@@ -13214,16 +13220,16 @@
       <c r="P165" s="5">
         <v>0.30380000000000001</v>
       </c>
-      <c r="Q165" s="7">
+      <c r="Q165" s="3">
         <v>68</v>
       </c>
-      <c r="R165" s="7">
+      <c r="R165" s="3">
         <v>81</v>
       </c>
-      <c r="S165" s="7">
+      <c r="S165" s="3">
         <v>2</v>
       </c>
-      <c r="T165" s="6">
+      <c r="T165" s="8">
         <v>1234.82</v>
       </c>
       <c r="U165" s="5">
@@ -13246,61 +13252,61 @@
       <c r="A166" s="4">
         <v>45211</v>
       </c>
-      <c r="B166" s="7">
+      <c r="B166" s="3">
         <v>72</v>
       </c>
-      <c r="C166" s="7">
+      <c r="C166" s="3">
         <v>141</v>
       </c>
-      <c r="D166" s="7">
-        <v>3</v>
-      </c>
-      <c r="E166" s="7">
+      <c r="D166" s="3">
+        <v>3</v>
+      </c>
+      <c r="E166" s="3">
         <v>22</v>
       </c>
       <c r="F166" s="5">
         <v>0.30559999999999998</v>
       </c>
-      <c r="G166" s="7">
+      <c r="G166" s="3">
         <v>29</v>
       </c>
-      <c r="H166" s="7">
-        <v>1</v>
-      </c>
-      <c r="I166" s="7">
+      <c r="H166" s="3">
+        <v>1</v>
+      </c>
+      <c r="I166" s="3">
         <v>26</v>
       </c>
-      <c r="J166" s="7">
+      <c r="J166" s="3">
         <v>30</v>
       </c>
       <c r="K166" s="5">
         <v>0.36109999999999998</v>
       </c>
-      <c r="L166" s="7">
+      <c r="L166" s="3">
         <v>4</v>
       </c>
-      <c r="M166" s="7">
+      <c r="M166" s="3">
         <v>4</v>
       </c>
-      <c r="N166" s="7">
-        <v>1</v>
-      </c>
-      <c r="O166" s="7">
+      <c r="N166" s="3">
+        <v>1</v>
+      </c>
+      <c r="O166" s="3">
         <v>97.6</v>
       </c>
       <c r="P166" s="5">
         <v>5.5599999999999997E-2</v>
       </c>
-      <c r="Q166" s="7">
+      <c r="Q166" s="3">
         <v>6</v>
       </c>
-      <c r="R166" s="7">
+      <c r="R166" s="3">
         <v>6</v>
       </c>
-      <c r="S166" s="7">
-        <v>1</v>
-      </c>
-      <c r="T166" s="7">
+      <c r="S166" s="3">
+        <v>1</v>
+      </c>
+      <c r="T166" s="8">
         <v>130.65</v>
       </c>
       <c r="U166" s="5">
@@ -13323,61 +13329,61 @@
       <c r="A167" s="4">
         <v>45212</v>
       </c>
-      <c r="B167" s="7">
+      <c r="B167" s="3">
         <v>117</v>
       </c>
-      <c r="C167" s="7">
+      <c r="C167" s="3">
         <v>265</v>
       </c>
-      <c r="D167" s="7">
-        <v>3</v>
-      </c>
-      <c r="E167" s="7">
+      <c r="D167" s="3">
+        <v>3</v>
+      </c>
+      <c r="E167" s="3">
         <v>22</v>
       </c>
       <c r="F167" s="5">
         <v>0.188</v>
       </c>
-      <c r="G167" s="7">
+      <c r="G167" s="3">
         <v>20</v>
       </c>
-      <c r="H167" s="7">
+      <c r="H167" s="3">
         <v>2</v>
       </c>
-      <c r="I167" s="7">
+      <c r="I167" s="3">
         <v>97</v>
       </c>
-      <c r="J167" s="7">
+      <c r="J167" s="3">
         <v>242</v>
       </c>
       <c r="K167" s="5">
         <v>0.82909999999999995</v>
       </c>
-      <c r="L167" s="7">
+      <c r="L167" s="3">
         <v>38</v>
       </c>
-      <c r="M167" s="7">
+      <c r="M167" s="3">
         <v>48</v>
       </c>
-      <c r="N167" s="7">
-        <v>1</v>
-      </c>
-      <c r="O167" s="7">
+      <c r="N167" s="3">
+        <v>1</v>
+      </c>
+      <c r="O167" s="3">
         <v>913.86</v>
       </c>
       <c r="P167" s="5">
         <v>0.32479999999999998</v>
       </c>
-      <c r="Q167" s="7">
+      <c r="Q167" s="3">
         <v>35</v>
       </c>
-      <c r="R167" s="7">
+      <c r="R167" s="3">
         <v>41</v>
       </c>
-      <c r="S167" s="7">
-        <v>1</v>
-      </c>
-      <c r="T167" s="7">
+      <c r="S167" s="3">
+        <v>1</v>
+      </c>
+      <c r="T167" s="8">
         <v>772.79</v>
       </c>
       <c r="U167" s="5">
@@ -13400,61 +13406,61 @@
       <c r="A168" s="4">
         <v>45213</v>
       </c>
-      <c r="B168" s="7">
+      <c r="B168" s="3">
         <v>91</v>
       </c>
-      <c r="C168" s="7">
+      <c r="C168" s="3">
         <v>183</v>
       </c>
-      <c r="D168" s="7">
-        <v>3</v>
-      </c>
-      <c r="E168" s="7">
+      <c r="D168" s="3">
+        <v>3</v>
+      </c>
+      <c r="E168" s="3">
         <v>19</v>
       </c>
       <c r="F168" s="5">
         <v>0.20880000000000001</v>
       </c>
-      <c r="G168" s="7">
+      <c r="G168" s="3">
         <v>27</v>
       </c>
-      <c r="H168" s="7">
-        <v>1</v>
-      </c>
-      <c r="I168" s="7">
+      <c r="H168" s="3">
+        <v>1</v>
+      </c>
+      <c r="I168" s="3">
         <v>62</v>
       </c>
-      <c r="J168" s="7">
+      <c r="J168" s="3">
         <v>99</v>
       </c>
       <c r="K168" s="5">
         <v>0.68130000000000002</v>
       </c>
-      <c r="L168" s="7">
+      <c r="L168" s="3">
         <v>22</v>
       </c>
-      <c r="M168" s="7">
+      <c r="M168" s="3">
         <v>29</v>
       </c>
-      <c r="N168" s="7">
-        <v>1</v>
-      </c>
-      <c r="O168" s="7">
+      <c r="N168" s="3">
+        <v>1</v>
+      </c>
+      <c r="O168" s="3">
         <v>540.13</v>
       </c>
       <c r="P168" s="5">
         <v>0.24179999999999999</v>
       </c>
-      <c r="Q168" s="7">
+      <c r="Q168" s="3">
         <v>20</v>
       </c>
-      <c r="R168" s="7">
+      <c r="R168" s="3">
         <v>27</v>
       </c>
-      <c r="S168" s="7">
-        <v>1</v>
-      </c>
-      <c r="T168" s="7">
+      <c r="S168" s="3">
+        <v>1</v>
+      </c>
+      <c r="T168" s="8">
         <v>503.93</v>
       </c>
       <c r="U168" s="5">
@@ -13477,61 +13483,61 @@
       <c r="A169" s="4">
         <v>45214</v>
       </c>
-      <c r="B169" s="7">
+      <c r="B169" s="3">
         <v>106</v>
       </c>
-      <c r="C169" s="7">
+      <c r="C169" s="3">
         <v>203</v>
       </c>
-      <c r="D169" s="7">
-        <v>3</v>
-      </c>
-      <c r="E169" s="7">
+      <c r="D169" s="3">
+        <v>3</v>
+      </c>
+      <c r="E169" s="3">
         <v>23</v>
       </c>
       <c r="F169" s="5">
         <v>0.217</v>
       </c>
-      <c r="G169" s="7">
+      <c r="G169" s="3">
         <v>34</v>
       </c>
-      <c r="H169" s="7">
-        <v>0</v>
-      </c>
-      <c r="I169" s="7">
+      <c r="H169" s="3">
+        <v>0</v>
+      </c>
+      <c r="I169" s="3">
         <v>43</v>
       </c>
-      <c r="J169" s="7">
+      <c r="J169" s="3">
         <v>63</v>
       </c>
       <c r="K169" s="5">
         <v>0.40570000000000001</v>
       </c>
-      <c r="L169" s="7">
+      <c r="L169" s="3">
         <v>8</v>
       </c>
-      <c r="M169" s="7">
+      <c r="M169" s="3">
         <v>8</v>
       </c>
-      <c r="N169" s="7">
-        <v>1</v>
-      </c>
-      <c r="O169" s="7">
+      <c r="N169" s="3">
+        <v>1</v>
+      </c>
+      <c r="O169" s="3">
         <v>133.97999999999999</v>
       </c>
       <c r="P169" s="5">
         <v>7.5499999999999998E-2</v>
       </c>
-      <c r="Q169" s="7">
+      <c r="Q169" s="3">
         <v>8</v>
       </c>
-      <c r="R169" s="7">
+      <c r="R169" s="3">
         <v>8</v>
       </c>
-      <c r="S169" s="7">
-        <v>1</v>
-      </c>
-      <c r="T169" s="7">
+      <c r="S169" s="3">
+        <v>1</v>
+      </c>
+      <c r="T169" s="8">
         <v>133.97999999999999</v>
       </c>
       <c r="U169" s="5">
@@ -13554,61 +13560,61 @@
       <c r="A170" s="4">
         <v>45215</v>
       </c>
-      <c r="B170" s="7">
+      <c r="B170" s="3">
         <v>102</v>
       </c>
-      <c r="C170" s="7">
+      <c r="C170" s="3">
         <v>172</v>
       </c>
-      <c r="D170" s="7">
-        <v>3</v>
-      </c>
-      <c r="E170" s="7">
+      <c r="D170" s="3">
+        <v>3</v>
+      </c>
+      <c r="E170" s="3">
         <v>25</v>
       </c>
       <c r="F170" s="5">
         <v>0.24510000000000001</v>
       </c>
-      <c r="G170" s="7">
+      <c r="G170" s="3">
         <v>17</v>
       </c>
-      <c r="H170" s="7">
-        <v>1</v>
-      </c>
-      <c r="I170" s="7">
+      <c r="H170" s="3">
+        <v>1</v>
+      </c>
+      <c r="I170" s="3">
         <v>28</v>
       </c>
-      <c r="J170" s="7">
+      <c r="J170" s="3">
         <v>33</v>
       </c>
       <c r="K170" s="5">
         <v>0.27450000000000002</v>
       </c>
-      <c r="L170" s="7">
+      <c r="L170" s="3">
         <v>6</v>
       </c>
-      <c r="M170" s="7">
+      <c r="M170" s="3">
         <v>6</v>
       </c>
-      <c r="N170" s="7">
-        <v>1</v>
-      </c>
-      <c r="O170" s="7">
+      <c r="N170" s="3">
+        <v>1</v>
+      </c>
+      <c r="O170" s="3">
         <v>181.8</v>
       </c>
       <c r="P170" s="5">
         <v>5.8799999999999998E-2</v>
       </c>
-      <c r="Q170" s="7">
+      <c r="Q170" s="3">
         <v>5</v>
       </c>
-      <c r="R170" s="7">
+      <c r="R170" s="3">
         <v>5</v>
       </c>
-      <c r="S170" s="7">
-        <v>1</v>
-      </c>
-      <c r="T170" s="7">
+      <c r="S170" s="3">
+        <v>1</v>
+      </c>
+      <c r="T170" s="8">
         <v>158.9</v>
       </c>
       <c r="U170" s="5">
@@ -13631,61 +13637,61 @@
       <c r="A171" s="4">
         <v>45216</v>
       </c>
-      <c r="B171" s="7">
+      <c r="B171" s="3">
         <v>87</v>
       </c>
-      <c r="C171" s="7">
+      <c r="C171" s="3">
         <v>189</v>
       </c>
-      <c r="D171" s="7">
-        <v>3</v>
-      </c>
-      <c r="E171" s="7">
+      <c r="D171" s="3">
+        <v>3</v>
+      </c>
+      <c r="E171" s="3">
         <v>21</v>
       </c>
       <c r="F171" s="5">
         <v>0.2414</v>
       </c>
-      <c r="G171" s="7">
+      <c r="G171" s="3">
         <v>22</v>
       </c>
-      <c r="H171" s="7">
-        <v>0</v>
-      </c>
-      <c r="I171" s="7">
+      <c r="H171" s="3">
+        <v>0</v>
+      </c>
+      <c r="I171" s="3">
         <v>48</v>
       </c>
-      <c r="J171" s="7">
+      <c r="J171" s="3">
         <v>72</v>
       </c>
       <c r="K171" s="5">
         <v>0.55169999999999997</v>
       </c>
-      <c r="L171" s="7">
+      <c r="L171" s="3">
         <v>11</v>
       </c>
-      <c r="M171" s="7">
+      <c r="M171" s="3">
         <v>12</v>
       </c>
-      <c r="N171" s="7">
-        <v>1</v>
-      </c>
-      <c r="O171" s="7">
+      <c r="N171" s="3">
+        <v>1</v>
+      </c>
+      <c r="O171" s="3">
         <v>232.85</v>
       </c>
       <c r="P171" s="5">
         <v>0.12640000000000001</v>
       </c>
-      <c r="Q171" s="7">
+      <c r="Q171" s="3">
         <v>9</v>
       </c>
-      <c r="R171" s="7">
+      <c r="R171" s="3">
         <v>10</v>
       </c>
-      <c r="S171" s="7">
-        <v>1</v>
-      </c>
-      <c r="T171" s="7">
+      <c r="S171" s="3">
+        <v>1</v>
+      </c>
+      <c r="T171" s="8">
         <v>196.65</v>
       </c>
       <c r="U171" s="5">
@@ -13708,61 +13714,61 @@
       <c r="A172" s="4">
         <v>45217</v>
       </c>
-      <c r="B172" s="7">
+      <c r="B172" s="3">
         <v>138</v>
       </c>
-      <c r="C172" s="7">
+      <c r="C172" s="3">
         <v>375</v>
       </c>
-      <c r="D172" s="7">
+      <c r="D172" s="3">
         <v>5</v>
       </c>
-      <c r="E172" s="7">
+      <c r="E172" s="3">
         <v>31</v>
       </c>
       <c r="F172" s="5">
         <v>0.22459999999999999</v>
       </c>
-      <c r="G172" s="7">
+      <c r="G172" s="3">
         <v>29</v>
       </c>
-      <c r="H172" s="7">
-        <v>1</v>
-      </c>
-      <c r="I172" s="7">
+      <c r="H172" s="3">
+        <v>1</v>
+      </c>
+      <c r="I172" s="3">
         <v>118</v>
       </c>
-      <c r="J172" s="7">
+      <c r="J172" s="3">
         <v>244</v>
       </c>
       <c r="K172" s="5">
         <v>0.85509999999999997</v>
       </c>
-      <c r="L172" s="7">
+      <c r="L172" s="3">
         <v>27</v>
       </c>
-      <c r="M172" s="7">
+      <c r="M172" s="3">
         <v>33</v>
       </c>
-      <c r="N172" s="7">
+      <c r="N172" s="3">
         <v>2</v>
       </c>
-      <c r="O172" s="7">
+      <c r="O172" s="3">
         <v>635.41</v>
       </c>
       <c r="P172" s="5">
         <v>0.19570000000000001</v>
       </c>
-      <c r="Q172" s="7">
+      <c r="Q172" s="3">
         <v>24</v>
       </c>
-      <c r="R172" s="7">
+      <c r="R172" s="3">
         <v>29</v>
       </c>
-      <c r="S172" s="7">
+      <c r="S172" s="3">
         <v>2</v>
       </c>
-      <c r="T172" s="7">
+      <c r="T172" s="8">
         <v>548.55999999999995</v>
       </c>
       <c r="U172" s="5">
@@ -13785,61 +13791,61 @@
       <c r="A173" s="4">
         <v>45218</v>
       </c>
-      <c r="B173" s="7">
+      <c r="B173" s="3">
         <v>68</v>
       </c>
-      <c r="C173" s="7">
+      <c r="C173" s="3">
         <v>121</v>
       </c>
-      <c r="D173" s="7">
-        <v>3</v>
-      </c>
-      <c r="E173" s="7">
+      <c r="D173" s="3">
+        <v>3</v>
+      </c>
+      <c r="E173" s="3">
         <v>15</v>
       </c>
       <c r="F173" s="5">
         <v>0.22059999999999999</v>
       </c>
-      <c r="G173" s="7">
+      <c r="G173" s="3">
         <v>10</v>
       </c>
-      <c r="H173" s="7">
-        <v>1</v>
-      </c>
-      <c r="I173" s="7">
+      <c r="H173" s="3">
+        <v>1</v>
+      </c>
+      <c r="I173" s="3">
         <v>43</v>
       </c>
-      <c r="J173" s="7">
+      <c r="J173" s="3">
         <v>73</v>
       </c>
       <c r="K173" s="5">
         <v>0.63239999999999996</v>
       </c>
-      <c r="L173" s="7">
+      <c r="L173" s="3">
         <v>10</v>
       </c>
-      <c r="M173" s="7">
+      <c r="M173" s="3">
         <v>10</v>
       </c>
-      <c r="N173" s="7">
-        <v>1</v>
-      </c>
-      <c r="O173" s="7">
+      <c r="N173" s="3">
+        <v>1</v>
+      </c>
+      <c r="O173" s="3">
         <v>199.8</v>
       </c>
       <c r="P173" s="5">
         <v>0.14710000000000001</v>
       </c>
-      <c r="Q173" s="7">
+      <c r="Q173" s="3">
         <v>8</v>
       </c>
-      <c r="R173" s="7">
+      <c r="R173" s="3">
         <v>8</v>
       </c>
-      <c r="S173" s="7">
-        <v>1</v>
-      </c>
-      <c r="T173" s="7">
+      <c r="S173" s="3">
+        <v>1</v>
+      </c>
+      <c r="T173" s="8">
         <v>146</v>
       </c>
       <c r="U173" s="5">
@@ -13862,61 +13868,61 @@
       <c r="A174" s="4">
         <v>45219</v>
       </c>
-      <c r="B174" s="7">
+      <c r="B174" s="3">
         <v>47</v>
       </c>
-      <c r="C174" s="7">
+      <c r="C174" s="3">
         <v>77</v>
       </c>
-      <c r="D174" s="7">
-        <v>3</v>
-      </c>
-      <c r="E174" s="7">
+      <c r="D174" s="3">
+        <v>3</v>
+      </c>
+      <c r="E174" s="3">
         <v>16</v>
       </c>
       <c r="F174" s="5">
         <v>0.34039999999999998</v>
       </c>
-      <c r="G174" s="7">
+      <c r="G174" s="3">
         <v>14</v>
       </c>
-      <c r="H174" s="7">
+      <c r="H174" s="3">
         <v>4</v>
       </c>
-      <c r="I174" s="7">
+      <c r="I174" s="3">
         <v>12</v>
       </c>
-      <c r="J174" s="7">
+      <c r="J174" s="3">
         <v>12</v>
       </c>
       <c r="K174" s="5">
         <v>0.25530000000000003</v>
       </c>
-      <c r="L174" s="7">
-        <v>0</v>
-      </c>
-      <c r="M174" s="7">
-        <v>0</v>
-      </c>
-      <c r="N174" s="7">
-        <v>0</v>
-      </c>
-      <c r="O174" s="7">
+      <c r="L174" s="3">
+        <v>0</v>
+      </c>
+      <c r="M174" s="3">
+        <v>0</v>
+      </c>
+      <c r="N174" s="3">
+        <v>0</v>
+      </c>
+      <c r="O174" s="3">
         <v>0</v>
       </c>
       <c r="P174" s="5">
         <v>0</v>
       </c>
-      <c r="Q174" s="7">
-        <v>1</v>
-      </c>
-      <c r="R174" s="7">
-        <v>1</v>
-      </c>
-      <c r="S174" s="7">
-        <v>1</v>
-      </c>
-      <c r="T174" s="7">
+      <c r="Q174" s="3">
+        <v>1</v>
+      </c>
+      <c r="R174" s="3">
+        <v>1</v>
+      </c>
+      <c r="S174" s="3">
+        <v>1</v>
+      </c>
+      <c r="T174" s="8">
         <v>22.9</v>
       </c>
       <c r="U174" s="5">
@@ -13939,61 +13945,61 @@
       <c r="A175" s="4">
         <v>45220</v>
       </c>
-      <c r="B175" s="7">
+      <c r="B175" s="3">
         <v>30</v>
       </c>
-      <c r="C175" s="7">
+      <c r="C175" s="3">
         <v>55</v>
       </c>
-      <c r="D175" s="7">
-        <v>3</v>
-      </c>
-      <c r="E175" s="7">
+      <c r="D175" s="3">
+        <v>3</v>
+      </c>
+      <c r="E175" s="3">
         <v>11</v>
       </c>
       <c r="F175" s="5">
         <v>0.36670000000000003</v>
       </c>
-      <c r="G175" s="7">
+      <c r="G175" s="3">
         <v>9</v>
       </c>
-      <c r="H175" s="7">
-        <v>1</v>
-      </c>
-      <c r="I175" s="7">
+      <c r="H175" s="3">
+        <v>1</v>
+      </c>
+      <c r="I175" s="3">
         <v>12</v>
       </c>
-      <c r="J175" s="7">
+      <c r="J175" s="3">
         <v>19</v>
       </c>
       <c r="K175" s="5">
         <v>0.4</v>
       </c>
-      <c r="L175" s="7">
-        <v>1</v>
-      </c>
-      <c r="M175" s="7">
-        <v>1</v>
-      </c>
-      <c r="N175" s="7">
-        <v>1</v>
-      </c>
-      <c r="O175" s="7">
+      <c r="L175" s="3">
+        <v>1</v>
+      </c>
+      <c r="M175" s="3">
+        <v>1</v>
+      </c>
+      <c r="N175" s="3">
+        <v>1</v>
+      </c>
+      <c r="O175" s="3">
         <v>10.9</v>
       </c>
       <c r="P175" s="5">
         <v>3.3300000000000003E-2</v>
       </c>
-      <c r="Q175" s="7">
-        <v>1</v>
-      </c>
-      <c r="R175" s="7">
-        <v>1</v>
-      </c>
-      <c r="S175" s="7">
-        <v>1</v>
-      </c>
-      <c r="T175" s="7">
+      <c r="Q175" s="3">
+        <v>1</v>
+      </c>
+      <c r="R175" s="3">
+        <v>1</v>
+      </c>
+      <c r="S175" s="3">
+        <v>1</v>
+      </c>
+      <c r="T175" s="8">
         <v>10.9</v>
       </c>
       <c r="U175" s="5">
@@ -14016,61 +14022,61 @@
       <c r="A176" s="4">
         <v>45221</v>
       </c>
-      <c r="B176" s="7">
+      <c r="B176" s="3">
         <v>56</v>
       </c>
-      <c r="C176" s="7">
+      <c r="C176" s="3">
         <v>109</v>
       </c>
-      <c r="D176" s="7">
+      <c r="D176" s="3">
         <v>4</v>
       </c>
-      <c r="E176" s="7">
+      <c r="E176" s="3">
         <v>12</v>
       </c>
       <c r="F176" s="5">
         <v>0.21429999999999999</v>
       </c>
-      <c r="G176" s="7">
+      <c r="G176" s="3">
         <v>17</v>
       </c>
-      <c r="H176" s="7">
-        <v>0</v>
-      </c>
-      <c r="I176" s="7">
+      <c r="H176" s="3">
+        <v>0</v>
+      </c>
+      <c r="I176" s="3">
         <v>30</v>
       </c>
-      <c r="J176" s="7">
+      <c r="J176" s="3">
         <v>40</v>
       </c>
       <c r="K176" s="5">
         <v>0.53569999999999995</v>
       </c>
-      <c r="L176" s="7">
+      <c r="L176" s="3">
         <v>2</v>
       </c>
-      <c r="M176" s="7">
+      <c r="M176" s="3">
         <v>2</v>
       </c>
-      <c r="N176" s="7">
-        <v>1</v>
-      </c>
-      <c r="O176" s="7">
+      <c r="N176" s="3">
+        <v>1</v>
+      </c>
+      <c r="O176" s="3">
         <v>19.8</v>
       </c>
       <c r="P176" s="5">
         <v>3.5700000000000003E-2</v>
       </c>
-      <c r="Q176" s="7">
+      <c r="Q176" s="3">
         <v>2</v>
       </c>
-      <c r="R176" s="7">
+      <c r="R176" s="3">
         <v>2</v>
       </c>
-      <c r="S176" s="7">
-        <v>1</v>
-      </c>
-      <c r="T176" s="7">
+      <c r="S176" s="3">
+        <v>1</v>
+      </c>
+      <c r="T176" s="8">
         <v>19.8</v>
       </c>
       <c r="U176" s="5">
@@ -14093,61 +14099,61 @@
       <c r="A177" s="4">
         <v>45222</v>
       </c>
-      <c r="B177" s="7">
+      <c r="B177" s="3">
         <v>61</v>
       </c>
-      <c r="C177" s="7">
+      <c r="C177" s="3">
         <v>110</v>
       </c>
-      <c r="D177" s="7">
-        <v>3</v>
-      </c>
-      <c r="E177" s="7">
+      <c r="D177" s="3">
+        <v>3</v>
+      </c>
+      <c r="E177" s="3">
         <v>11</v>
       </c>
       <c r="F177" s="5">
         <v>0.18029999999999999</v>
       </c>
-      <c r="G177" s="7">
+      <c r="G177" s="3">
         <v>13</v>
       </c>
-      <c r="H177" s="7">
-        <v>0</v>
-      </c>
-      <c r="I177" s="7">
+      <c r="H177" s="3">
+        <v>0</v>
+      </c>
+      <c r="I177" s="3">
         <v>32</v>
       </c>
-      <c r="J177" s="7">
+      <c r="J177" s="3">
         <v>39</v>
       </c>
       <c r="K177" s="5">
         <v>0.52459999999999996</v>
       </c>
-      <c r="L177" s="7">
-        <v>3</v>
-      </c>
-      <c r="M177" s="7">
-        <v>3</v>
-      </c>
-      <c r="N177" s="7">
-        <v>1</v>
-      </c>
-      <c r="O177" s="7">
+      <c r="L177" s="3">
+        <v>3</v>
+      </c>
+      <c r="M177" s="3">
+        <v>3</v>
+      </c>
+      <c r="N177" s="3">
+        <v>1</v>
+      </c>
+      <c r="O177" s="3">
         <v>69.66</v>
       </c>
       <c r="P177" s="5">
         <v>4.9200000000000001E-2</v>
       </c>
-      <c r="Q177" s="7">
-        <v>3</v>
-      </c>
-      <c r="R177" s="7">
-        <v>3</v>
-      </c>
-      <c r="S177" s="7">
-        <v>1</v>
-      </c>
-      <c r="T177" s="7">
+      <c r="Q177" s="3">
+        <v>3</v>
+      </c>
+      <c r="R177" s="3">
+        <v>3</v>
+      </c>
+      <c r="S177" s="3">
+        <v>1</v>
+      </c>
+      <c r="T177" s="8">
         <v>69.66</v>
       </c>
       <c r="U177" s="5">
@@ -14170,61 +14176,61 @@
       <c r="A178" s="4">
         <v>45223</v>
       </c>
-      <c r="B178" s="7">
+      <c r="B178" s="3">
         <v>70</v>
       </c>
-      <c r="C178" s="7">
+      <c r="C178" s="3">
         <v>142</v>
       </c>
-      <c r="D178" s="7">
-        <v>3</v>
-      </c>
-      <c r="E178" s="7">
+      <c r="D178" s="3">
+        <v>3</v>
+      </c>
+      <c r="E178" s="3">
         <v>23</v>
       </c>
       <c r="F178" s="5">
         <v>0.3286</v>
       </c>
-      <c r="G178" s="7">
+      <c r="G178" s="3">
         <v>20</v>
       </c>
-      <c r="H178" s="7">
-        <v>1</v>
-      </c>
-      <c r="I178" s="7">
+      <c r="H178" s="3">
+        <v>1</v>
+      </c>
+      <c r="I178" s="3">
         <v>16</v>
       </c>
-      <c r="J178" s="7">
+      <c r="J178" s="3">
         <v>18</v>
       </c>
       <c r="K178" s="5">
         <v>0.2286</v>
       </c>
-      <c r="L178" s="7">
+      <c r="L178" s="3">
         <v>4</v>
       </c>
-      <c r="M178" s="7">
+      <c r="M178" s="3">
         <v>4</v>
       </c>
-      <c r="N178" s="7">
-        <v>1</v>
-      </c>
-      <c r="O178" s="7">
+      <c r="N178" s="3">
+        <v>1</v>
+      </c>
+      <c r="O178" s="3">
         <v>61.6</v>
       </c>
       <c r="P178" s="5">
         <v>5.7099999999999998E-2</v>
       </c>
-      <c r="Q178" s="7">
+      <c r="Q178" s="3">
         <v>4</v>
       </c>
-      <c r="R178" s="7">
+      <c r="R178" s="3">
         <v>4</v>
       </c>
-      <c r="S178" s="7">
-        <v>1</v>
-      </c>
-      <c r="T178" s="7">
+      <c r="S178" s="3">
+        <v>1</v>
+      </c>
+      <c r="T178" s="8">
         <v>61.6</v>
       </c>
       <c r="U178" s="5">
@@ -14247,43 +14253,43 @@
       <c r="A179" s="4">
         <v>45224</v>
       </c>
-      <c r="B179" s="7">
+      <c r="B179" s="3">
         <v>142</v>
       </c>
-      <c r="C179" s="7">
+      <c r="C179" s="3">
         <v>360</v>
       </c>
-      <c r="D179" s="7">
-        <v>3</v>
-      </c>
-      <c r="E179" s="7">
+      <c r="D179" s="3">
+        <v>3</v>
+      </c>
+      <c r="E179" s="3">
         <v>25</v>
       </c>
       <c r="F179" s="5">
         <v>0.17610000000000001</v>
       </c>
-      <c r="G179" s="7">
+      <c r="G179" s="3">
         <v>37</v>
       </c>
-      <c r="H179" s="7">
+      <c r="H179" s="3">
         <v>2</v>
       </c>
-      <c r="I179" s="7">
+      <c r="I179" s="3">
         <v>171</v>
       </c>
-      <c r="J179" s="7">
+      <c r="J179" s="3">
         <v>356</v>
       </c>
       <c r="K179" s="5">
         <v>1.2041999999999999</v>
       </c>
-      <c r="L179" s="7">
+      <c r="L179" s="3">
         <v>62</v>
       </c>
-      <c r="M179" s="7">
+      <c r="M179" s="3">
         <v>66</v>
       </c>
-      <c r="N179" s="7">
+      <c r="N179" s="3">
         <v>2</v>
       </c>
       <c r="O179" s="6">
@@ -14292,16 +14298,16 @@
       <c r="P179" s="5">
         <v>0.43659999999999999</v>
       </c>
-      <c r="Q179" s="7">
+      <c r="Q179" s="3">
         <v>60</v>
       </c>
-      <c r="R179" s="7">
+      <c r="R179" s="3">
         <v>63</v>
       </c>
-      <c r="S179" s="7">
+      <c r="S179" s="3">
         <v>2</v>
       </c>
-      <c r="T179" s="6">
+      <c r="T179" s="8">
         <v>1198.8800000000001</v>
       </c>
       <c r="U179" s="5">
@@ -14324,61 +14330,61 @@
       <c r="A180" s="4">
         <v>45225</v>
       </c>
-      <c r="B180" s="7">
+      <c r="B180" s="3">
         <v>108</v>
       </c>
-      <c r="C180" s="7">
+      <c r="C180" s="3">
         <v>221</v>
       </c>
-      <c r="D180" s="7">
+      <c r="D180" s="3">
         <v>4</v>
       </c>
-      <c r="E180" s="7">
+      <c r="E180" s="3">
         <v>27</v>
       </c>
       <c r="F180" s="5">
         <v>0.25</v>
       </c>
-      <c r="G180" s="7">
+      <c r="G180" s="3">
         <v>17</v>
       </c>
-      <c r="H180" s="7">
-        <v>1</v>
-      </c>
-      <c r="I180" s="7">
+      <c r="H180" s="3">
+        <v>1</v>
+      </c>
+      <c r="I180" s="3">
         <v>77</v>
       </c>
-      <c r="J180" s="7">
+      <c r="J180" s="3">
         <v>115</v>
       </c>
       <c r="K180" s="5">
         <v>0.71299999999999997</v>
       </c>
-      <c r="L180" s="7">
+      <c r="L180" s="3">
         <v>23</v>
       </c>
-      <c r="M180" s="7">
+      <c r="M180" s="3">
         <v>25</v>
       </c>
-      <c r="N180" s="7">
-        <v>1</v>
-      </c>
-      <c r="O180" s="7">
+      <c r="N180" s="3">
+        <v>1</v>
+      </c>
+      <c r="O180" s="3">
         <v>497.05</v>
       </c>
       <c r="P180" s="5">
         <v>0.21299999999999999</v>
       </c>
-      <c r="Q180" s="7">
+      <c r="Q180" s="3">
         <v>21</v>
       </c>
-      <c r="R180" s="7">
+      <c r="R180" s="3">
         <v>23</v>
       </c>
-      <c r="S180" s="7">
-        <v>1</v>
-      </c>
-      <c r="T180" s="7">
+      <c r="S180" s="3">
+        <v>1</v>
+      </c>
+      <c r="T180" s="8">
         <v>471.25</v>
       </c>
       <c r="U180" s="5">
@@ -14401,61 +14407,61 @@
       <c r="A181" s="4">
         <v>45226</v>
       </c>
-      <c r="B181" s="7">
+      <c r="B181" s="3">
         <v>74</v>
       </c>
-      <c r="C181" s="7">
+      <c r="C181" s="3">
         <v>180</v>
       </c>
-      <c r="D181" s="7">
+      <c r="D181" s="3">
         <v>4</v>
       </c>
-      <c r="E181" s="7">
+      <c r="E181" s="3">
         <v>13</v>
       </c>
       <c r="F181" s="5">
         <v>0.1757</v>
       </c>
-      <c r="G181" s="7">
+      <c r="G181" s="3">
         <v>19</v>
       </c>
-      <c r="H181" s="7">
-        <v>1</v>
-      </c>
-      <c r="I181" s="7">
+      <c r="H181" s="3">
+        <v>1</v>
+      </c>
+      <c r="I181" s="3">
         <v>56</v>
       </c>
-      <c r="J181" s="7">
+      <c r="J181" s="3">
         <v>108</v>
       </c>
       <c r="K181" s="5">
         <v>0.75680000000000003</v>
       </c>
-      <c r="L181" s="7">
+      <c r="L181" s="3">
         <v>21</v>
       </c>
-      <c r="M181" s="7">
+      <c r="M181" s="3">
         <v>32</v>
       </c>
-      <c r="N181" s="7">
-        <v>1</v>
-      </c>
-      <c r="O181" s="7">
+      <c r="N181" s="3">
+        <v>1</v>
+      </c>
+      <c r="O181" s="3">
         <v>548.83000000000004</v>
       </c>
       <c r="P181" s="5">
         <v>0.2838</v>
       </c>
-      <c r="Q181" s="7">
+      <c r="Q181" s="3">
         <v>19</v>
       </c>
-      <c r="R181" s="7">
+      <c r="R181" s="3">
         <v>27</v>
       </c>
-      <c r="S181" s="7">
-        <v>1</v>
-      </c>
-      <c r="T181" s="7">
+      <c r="S181" s="3">
+        <v>1</v>
+      </c>
+      <c r="T181" s="8">
         <v>469.23</v>
       </c>
       <c r="U181" s="5">
@@ -14478,61 +14484,61 @@
       <c r="A182" s="4">
         <v>45227</v>
       </c>
-      <c r="B182" s="7">
+      <c r="B182" s="3">
         <v>53</v>
       </c>
-      <c r="C182" s="7">
+      <c r="C182" s="3">
         <v>86</v>
       </c>
-      <c r="D182" s="7">
-        <v>3</v>
-      </c>
-      <c r="E182" s="7">
+      <c r="D182" s="3">
+        <v>3</v>
+      </c>
+      <c r="E182" s="3">
         <v>16</v>
       </c>
       <c r="F182" s="5">
         <v>0.3019</v>
       </c>
-      <c r="G182" s="7">
+      <c r="G182" s="3">
         <v>10</v>
       </c>
-      <c r="H182" s="7">
-        <v>1</v>
-      </c>
-      <c r="I182" s="7">
+      <c r="H182" s="3">
+        <v>1</v>
+      </c>
+      <c r="I182" s="3">
         <v>15</v>
       </c>
-      <c r="J182" s="7">
+      <c r="J182" s="3">
         <v>17</v>
       </c>
       <c r="K182" s="5">
         <v>0.28299999999999997</v>
       </c>
-      <c r="L182" s="7">
+      <c r="L182" s="3">
         <v>2</v>
       </c>
-      <c r="M182" s="7">
+      <c r="M182" s="3">
         <v>2</v>
       </c>
-      <c r="N182" s="7">
-        <v>1</v>
-      </c>
-      <c r="O182" s="7">
+      <c r="N182" s="3">
+        <v>1</v>
+      </c>
+      <c r="O182" s="3">
         <v>25.8</v>
       </c>
       <c r="P182" s="5">
         <v>3.7699999999999997E-2</v>
       </c>
-      <c r="Q182" s="7">
+      <c r="Q182" s="3">
         <v>2</v>
       </c>
-      <c r="R182" s="7">
+      <c r="R182" s="3">
         <v>2</v>
       </c>
-      <c r="S182" s="7">
-        <v>1</v>
-      </c>
-      <c r="T182" s="7">
+      <c r="S182" s="3">
+        <v>1</v>
+      </c>
+      <c r="T182" s="8">
         <v>25.8</v>
       </c>
       <c r="U182" s="5">
@@ -14555,61 +14561,61 @@
       <c r="A183" s="4">
         <v>45228</v>
       </c>
-      <c r="B183" s="7">
+      <c r="B183" s="3">
         <v>78</v>
       </c>
-      <c r="C183" s="7">
+      <c r="C183" s="3">
         <v>133</v>
       </c>
-      <c r="D183" s="7">
-        <v>3</v>
-      </c>
-      <c r="E183" s="7">
+      <c r="D183" s="3">
+        <v>3</v>
+      </c>
+      <c r="E183" s="3">
         <v>29</v>
       </c>
       <c r="F183" s="5">
         <v>0.37180000000000002</v>
       </c>
-      <c r="G183" s="7">
+      <c r="G183" s="3">
         <v>30</v>
       </c>
-      <c r="H183" s="7">
-        <v>0</v>
-      </c>
-      <c r="I183" s="7">
+      <c r="H183" s="3">
+        <v>0</v>
+      </c>
+      <c r="I183" s="3">
         <v>11</v>
       </c>
-      <c r="J183" s="7">
+      <c r="J183" s="3">
         <v>12</v>
       </c>
       <c r="K183" s="5">
         <v>0.14099999999999999</v>
       </c>
-      <c r="L183" s="7">
+      <c r="L183" s="3">
         <v>5</v>
       </c>
-      <c r="M183" s="7">
+      <c r="M183" s="3">
         <v>6</v>
       </c>
-      <c r="N183" s="7">
-        <v>1</v>
-      </c>
-      <c r="O183" s="7">
+      <c r="N183" s="3">
+        <v>1</v>
+      </c>
+      <c r="O183" s="3">
         <v>140.9</v>
       </c>
       <c r="P183" s="5">
         <v>6.4100000000000004E-2</v>
       </c>
-      <c r="Q183" s="7">
+      <c r="Q183" s="3">
         <v>5</v>
       </c>
-      <c r="R183" s="7">
+      <c r="R183" s="3">
         <v>6</v>
       </c>
-      <c r="S183" s="7">
-        <v>1</v>
-      </c>
-      <c r="T183" s="7">
+      <c r="S183" s="3">
+        <v>1</v>
+      </c>
+      <c r="T183" s="8">
         <v>140.9</v>
       </c>
       <c r="U183" s="5">
@@ -14632,61 +14638,61 @@
       <c r="A184" s="4">
         <v>45229</v>
       </c>
-      <c r="B184" s="7">
+      <c r="B184" s="3">
         <v>88</v>
       </c>
-      <c r="C184" s="7">
+      <c r="C184" s="3">
         <v>144</v>
       </c>
-      <c r="D184" s="7">
-        <v>3</v>
-      </c>
-      <c r="E184" s="7">
+      <c r="D184" s="3">
+        <v>3</v>
+      </c>
+      <c r="E184" s="3">
         <v>29</v>
       </c>
       <c r="F184" s="5">
         <v>0.32950000000000002</v>
       </c>
-      <c r="G184" s="7">
+      <c r="G184" s="3">
         <v>33</v>
       </c>
-      <c r="H184" s="7">
-        <v>3</v>
-      </c>
-      <c r="I184" s="7">
+      <c r="H184" s="3">
+        <v>3</v>
+      </c>
+      <c r="I184" s="3">
         <v>29</v>
       </c>
-      <c r="J184" s="7">
+      <c r="J184" s="3">
         <v>36</v>
       </c>
       <c r="K184" s="5">
         <v>0.32950000000000002</v>
       </c>
-      <c r="L184" s="7">
+      <c r="L184" s="3">
         <v>11</v>
       </c>
-      <c r="M184" s="7">
+      <c r="M184" s="3">
         <v>12</v>
       </c>
-      <c r="N184" s="7">
-        <v>1</v>
-      </c>
-      <c r="O184" s="7">
+      <c r="N184" s="3">
+        <v>1</v>
+      </c>
+      <c r="O184" s="3">
         <v>313.81</v>
       </c>
       <c r="P184" s="5">
         <v>0.125</v>
       </c>
-      <c r="Q184" s="7">
+      <c r="Q184" s="3">
         <v>11</v>
       </c>
-      <c r="R184" s="7">
+      <c r="R184" s="3">
         <v>12</v>
       </c>
-      <c r="S184" s="7">
-        <v>1</v>
-      </c>
-      <c r="T184" s="7">
+      <c r="S184" s="3">
+        <v>1</v>
+      </c>
+      <c r="T184" s="8">
         <v>313.81</v>
       </c>
       <c r="U184" s="5">
@@ -14709,61 +14715,61 @@
       <c r="A185" s="4">
         <v>45230</v>
       </c>
-      <c r="B185" s="7">
+      <c r="B185" s="3">
         <v>122</v>
       </c>
-      <c r="C185" s="7">
+      <c r="C185" s="3">
         <v>282</v>
       </c>
-      <c r="D185" s="7">
+      <c r="D185" s="3">
         <v>4</v>
       </c>
-      <c r="E185" s="7">
+      <c r="E185" s="3">
         <v>24</v>
       </c>
       <c r="F185" s="5">
         <v>0.19670000000000001</v>
       </c>
-      <c r="G185" s="7">
+      <c r="G185" s="3">
         <v>43</v>
       </c>
-      <c r="H185" s="7">
-        <v>3</v>
-      </c>
-      <c r="I185" s="7">
+      <c r="H185" s="3">
+        <v>3</v>
+      </c>
+      <c r="I185" s="3">
         <v>60</v>
       </c>
-      <c r="J185" s="7">
+      <c r="J185" s="3">
         <v>169</v>
       </c>
       <c r="K185" s="5">
         <v>0.49180000000000001</v>
       </c>
-      <c r="L185" s="7">
+      <c r="L185" s="3">
         <v>15</v>
       </c>
-      <c r="M185" s="7">
+      <c r="M185" s="3">
         <v>26</v>
       </c>
-      <c r="N185" s="7">
+      <c r="N185" s="3">
         <v>2</v>
       </c>
-      <c r="O185" s="7">
+      <c r="O185" s="3">
         <v>743.54</v>
       </c>
       <c r="P185" s="5">
         <v>0.123</v>
       </c>
-      <c r="Q185" s="7">
+      <c r="Q185" s="3">
         <v>15</v>
       </c>
-      <c r="R185" s="7">
+      <c r="R185" s="3">
         <v>21</v>
       </c>
-      <c r="S185" s="7">
+      <c r="S185" s="3">
         <v>2</v>
       </c>
-      <c r="T185" s="7">
+      <c r="T185" s="8">
         <v>571.94000000000005</v>
       </c>
       <c r="U185" s="5">

</xml_diff>